<commit_message>
added Zone as a feature and fixed rounding issues in preview of data
</commit_message>
<xml_diff>
--- a/FORMAT_WORBYN.xlsx
+++ b/FORMAT_WORBYN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shri Karthik\Desktop\DIAGRAM-MAPPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56429C8A-52D5-4DEF-8B7A-56E6382FFBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CB3413-7199-4ABE-BFC3-6476054128BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAIR" sheetId="2" r:id="rId1"/>
@@ -124,7 +124,7 @@
     <definedName name="_Dist_Bin" hidden="1">#REF!</definedName>
     <definedName name="_Dist_Values" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">'[5]SAMPLE HISTOGRAM'!$P$19:$P$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FAIR!$A$11:$H$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FAIR!$A$11:$H$57</definedName>
     <definedName name="_FLD1">#REF!</definedName>
     <definedName name="_FLD2">#REF!</definedName>
     <definedName name="_FLD3">#REF!</definedName>
@@ -1002,7 +1002,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,6 +1082,82 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1114,93 +1190,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1220,6 +1214,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7094,834 +7100,834 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC194"/>
+  <dimension ref="A1:AC193"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57:C57"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" style="9" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="15" max="249" width="8.85546875" style="3"/>
-    <col min="250" max="250" width="4.7109375" style="3" customWidth="1"/>
-    <col min="251" max="251" width="5.28515625" style="3" customWidth="1"/>
-    <col min="252" max="252" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" style="9" customWidth="1"/>
+    <col min="10" max="11" width="11.5546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="15" max="249" width="8.88671875" style="3"/>
+    <col min="250" max="250" width="4.6640625" style="3" customWidth="1"/>
+    <col min="251" max="251" width="5.33203125" style="3" customWidth="1"/>
+    <col min="252" max="252" width="6.88671875" style="3" customWidth="1"/>
     <col min="253" max="253" width="18" style="3" customWidth="1"/>
-    <col min="254" max="254" width="30.7109375" style="3" customWidth="1"/>
-    <col min="255" max="256" width="9.140625" style="3" customWidth="1"/>
-    <col min="257" max="257" width="21.5703125" style="3" customWidth="1"/>
-    <col min="258" max="258" width="11.5703125" style="3" customWidth="1"/>
-    <col min="259" max="259" width="10.5703125" style="3" customWidth="1"/>
-    <col min="260" max="260" width="12.28515625" style="3" customWidth="1"/>
-    <col min="261" max="505" width="8.85546875" style="3"/>
-    <col min="506" max="506" width="4.7109375" style="3" customWidth="1"/>
-    <col min="507" max="507" width="5.28515625" style="3" customWidth="1"/>
-    <col min="508" max="508" width="6.85546875" style="3" customWidth="1"/>
+    <col min="254" max="254" width="30.6640625" style="3" customWidth="1"/>
+    <col min="255" max="256" width="9.109375" style="3" customWidth="1"/>
+    <col min="257" max="257" width="21.5546875" style="3" customWidth="1"/>
+    <col min="258" max="258" width="11.5546875" style="3" customWidth="1"/>
+    <col min="259" max="259" width="10.5546875" style="3" customWidth="1"/>
+    <col min="260" max="260" width="12.33203125" style="3" customWidth="1"/>
+    <col min="261" max="505" width="8.88671875" style="3"/>
+    <col min="506" max="506" width="4.6640625" style="3" customWidth="1"/>
+    <col min="507" max="507" width="5.33203125" style="3" customWidth="1"/>
+    <col min="508" max="508" width="6.88671875" style="3" customWidth="1"/>
     <col min="509" max="509" width="18" style="3" customWidth="1"/>
-    <col min="510" max="510" width="30.7109375" style="3" customWidth="1"/>
-    <col min="511" max="512" width="9.140625" style="3" customWidth="1"/>
-    <col min="513" max="513" width="21.5703125" style="3" customWidth="1"/>
-    <col min="514" max="514" width="11.5703125" style="3" customWidth="1"/>
-    <col min="515" max="515" width="10.5703125" style="3" customWidth="1"/>
-    <col min="516" max="516" width="12.28515625" style="3" customWidth="1"/>
-    <col min="517" max="761" width="8.85546875" style="3"/>
-    <col min="762" max="762" width="4.7109375" style="3" customWidth="1"/>
-    <col min="763" max="763" width="5.28515625" style="3" customWidth="1"/>
-    <col min="764" max="764" width="6.85546875" style="3" customWidth="1"/>
+    <col min="510" max="510" width="30.6640625" style="3" customWidth="1"/>
+    <col min="511" max="512" width="9.109375" style="3" customWidth="1"/>
+    <col min="513" max="513" width="21.5546875" style="3" customWidth="1"/>
+    <col min="514" max="514" width="11.5546875" style="3" customWidth="1"/>
+    <col min="515" max="515" width="10.5546875" style="3" customWidth="1"/>
+    <col min="516" max="516" width="12.33203125" style="3" customWidth="1"/>
+    <col min="517" max="761" width="8.88671875" style="3"/>
+    <col min="762" max="762" width="4.6640625" style="3" customWidth="1"/>
+    <col min="763" max="763" width="5.33203125" style="3" customWidth="1"/>
+    <col min="764" max="764" width="6.88671875" style="3" customWidth="1"/>
     <col min="765" max="765" width="18" style="3" customWidth="1"/>
-    <col min="766" max="766" width="30.7109375" style="3" customWidth="1"/>
-    <col min="767" max="768" width="9.140625" style="3" customWidth="1"/>
-    <col min="769" max="769" width="21.5703125" style="3" customWidth="1"/>
-    <col min="770" max="770" width="11.5703125" style="3" customWidth="1"/>
-    <col min="771" max="771" width="10.5703125" style="3" customWidth="1"/>
-    <col min="772" max="772" width="12.28515625" style="3" customWidth="1"/>
-    <col min="773" max="1017" width="8.85546875" style="3"/>
-    <col min="1018" max="1018" width="4.7109375" style="3" customWidth="1"/>
-    <col min="1019" max="1019" width="5.28515625" style="3" customWidth="1"/>
-    <col min="1020" max="1020" width="6.85546875" style="3" customWidth="1"/>
+    <col min="766" max="766" width="30.6640625" style="3" customWidth="1"/>
+    <col min="767" max="768" width="9.109375" style="3" customWidth="1"/>
+    <col min="769" max="769" width="21.5546875" style="3" customWidth="1"/>
+    <col min="770" max="770" width="11.5546875" style="3" customWidth="1"/>
+    <col min="771" max="771" width="10.5546875" style="3" customWidth="1"/>
+    <col min="772" max="772" width="12.33203125" style="3" customWidth="1"/>
+    <col min="773" max="1017" width="8.88671875" style="3"/>
+    <col min="1018" max="1018" width="4.6640625" style="3" customWidth="1"/>
+    <col min="1019" max="1019" width="5.33203125" style="3" customWidth="1"/>
+    <col min="1020" max="1020" width="6.88671875" style="3" customWidth="1"/>
     <col min="1021" max="1021" width="18" style="3" customWidth="1"/>
-    <col min="1022" max="1022" width="30.7109375" style="3" customWidth="1"/>
-    <col min="1023" max="1024" width="9.140625" style="3" customWidth="1"/>
-    <col min="1025" max="1025" width="21.5703125" style="3" customWidth="1"/>
-    <col min="1026" max="1026" width="11.5703125" style="3" customWidth="1"/>
-    <col min="1027" max="1027" width="10.5703125" style="3" customWidth="1"/>
-    <col min="1028" max="1028" width="12.28515625" style="3" customWidth="1"/>
-    <col min="1029" max="1273" width="8.85546875" style="3"/>
-    <col min="1274" max="1274" width="4.7109375" style="3" customWidth="1"/>
-    <col min="1275" max="1275" width="5.28515625" style="3" customWidth="1"/>
-    <col min="1276" max="1276" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1022" max="1022" width="30.6640625" style="3" customWidth="1"/>
+    <col min="1023" max="1024" width="9.109375" style="3" customWidth="1"/>
+    <col min="1025" max="1025" width="21.5546875" style="3" customWidth="1"/>
+    <col min="1026" max="1026" width="11.5546875" style="3" customWidth="1"/>
+    <col min="1027" max="1027" width="10.5546875" style="3" customWidth="1"/>
+    <col min="1028" max="1028" width="12.33203125" style="3" customWidth="1"/>
+    <col min="1029" max="1273" width="8.88671875" style="3"/>
+    <col min="1274" max="1274" width="4.6640625" style="3" customWidth="1"/>
+    <col min="1275" max="1275" width="5.33203125" style="3" customWidth="1"/>
+    <col min="1276" max="1276" width="6.88671875" style="3" customWidth="1"/>
     <col min="1277" max="1277" width="18" style="3" customWidth="1"/>
-    <col min="1278" max="1278" width="30.7109375" style="3" customWidth="1"/>
-    <col min="1279" max="1280" width="9.140625" style="3" customWidth="1"/>
-    <col min="1281" max="1281" width="21.5703125" style="3" customWidth="1"/>
-    <col min="1282" max="1282" width="11.5703125" style="3" customWidth="1"/>
-    <col min="1283" max="1283" width="10.5703125" style="3" customWidth="1"/>
-    <col min="1284" max="1284" width="12.28515625" style="3" customWidth="1"/>
-    <col min="1285" max="1529" width="8.85546875" style="3"/>
-    <col min="1530" max="1530" width="4.7109375" style="3" customWidth="1"/>
-    <col min="1531" max="1531" width="5.28515625" style="3" customWidth="1"/>
-    <col min="1532" max="1532" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1278" max="1278" width="30.6640625" style="3" customWidth="1"/>
+    <col min="1279" max="1280" width="9.109375" style="3" customWidth="1"/>
+    <col min="1281" max="1281" width="21.5546875" style="3" customWidth="1"/>
+    <col min="1282" max="1282" width="11.5546875" style="3" customWidth="1"/>
+    <col min="1283" max="1283" width="10.5546875" style="3" customWidth="1"/>
+    <col min="1284" max="1284" width="12.33203125" style="3" customWidth="1"/>
+    <col min="1285" max="1529" width="8.88671875" style="3"/>
+    <col min="1530" max="1530" width="4.6640625" style="3" customWidth="1"/>
+    <col min="1531" max="1531" width="5.33203125" style="3" customWidth="1"/>
+    <col min="1532" max="1532" width="6.88671875" style="3" customWidth="1"/>
     <col min="1533" max="1533" width="18" style="3" customWidth="1"/>
-    <col min="1534" max="1534" width="30.7109375" style="3" customWidth="1"/>
-    <col min="1535" max="1536" width="9.140625" style="3" customWidth="1"/>
-    <col min="1537" max="1537" width="21.5703125" style="3" customWidth="1"/>
-    <col min="1538" max="1538" width="11.5703125" style="3" customWidth="1"/>
-    <col min="1539" max="1539" width="10.5703125" style="3" customWidth="1"/>
-    <col min="1540" max="1540" width="12.28515625" style="3" customWidth="1"/>
-    <col min="1541" max="1785" width="8.85546875" style="3"/>
-    <col min="1786" max="1786" width="4.7109375" style="3" customWidth="1"/>
-    <col min="1787" max="1787" width="5.28515625" style="3" customWidth="1"/>
-    <col min="1788" max="1788" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1534" max="1534" width="30.6640625" style="3" customWidth="1"/>
+    <col min="1535" max="1536" width="9.109375" style="3" customWidth="1"/>
+    <col min="1537" max="1537" width="21.5546875" style="3" customWidth="1"/>
+    <col min="1538" max="1538" width="11.5546875" style="3" customWidth="1"/>
+    <col min="1539" max="1539" width="10.5546875" style="3" customWidth="1"/>
+    <col min="1540" max="1540" width="12.33203125" style="3" customWidth="1"/>
+    <col min="1541" max="1785" width="8.88671875" style="3"/>
+    <col min="1786" max="1786" width="4.6640625" style="3" customWidth="1"/>
+    <col min="1787" max="1787" width="5.33203125" style="3" customWidth="1"/>
+    <col min="1788" max="1788" width="6.88671875" style="3" customWidth="1"/>
     <col min="1789" max="1789" width="18" style="3" customWidth="1"/>
-    <col min="1790" max="1790" width="30.7109375" style="3" customWidth="1"/>
-    <col min="1791" max="1792" width="9.140625" style="3" customWidth="1"/>
-    <col min="1793" max="1793" width="21.5703125" style="3" customWidth="1"/>
-    <col min="1794" max="1794" width="11.5703125" style="3" customWidth="1"/>
-    <col min="1795" max="1795" width="10.5703125" style="3" customWidth="1"/>
-    <col min="1796" max="1796" width="12.28515625" style="3" customWidth="1"/>
-    <col min="1797" max="2041" width="8.85546875" style="3"/>
-    <col min="2042" max="2042" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2043" max="2043" width="5.28515625" style="3" customWidth="1"/>
-    <col min="2044" max="2044" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1790" max="1790" width="30.6640625" style="3" customWidth="1"/>
+    <col min="1791" max="1792" width="9.109375" style="3" customWidth="1"/>
+    <col min="1793" max="1793" width="21.5546875" style="3" customWidth="1"/>
+    <col min="1794" max="1794" width="11.5546875" style="3" customWidth="1"/>
+    <col min="1795" max="1795" width="10.5546875" style="3" customWidth="1"/>
+    <col min="1796" max="1796" width="12.33203125" style="3" customWidth="1"/>
+    <col min="1797" max="2041" width="8.88671875" style="3"/>
+    <col min="2042" max="2042" width="4.6640625" style="3" customWidth="1"/>
+    <col min="2043" max="2043" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2044" max="2044" width="6.88671875" style="3" customWidth="1"/>
     <col min="2045" max="2045" width="18" style="3" customWidth="1"/>
-    <col min="2046" max="2046" width="30.7109375" style="3" customWidth="1"/>
-    <col min="2047" max="2048" width="9.140625" style="3" customWidth="1"/>
-    <col min="2049" max="2049" width="21.5703125" style="3" customWidth="1"/>
-    <col min="2050" max="2050" width="11.5703125" style="3" customWidth="1"/>
-    <col min="2051" max="2051" width="10.5703125" style="3" customWidth="1"/>
-    <col min="2052" max="2052" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2053" max="2297" width="8.85546875" style="3"/>
-    <col min="2298" max="2298" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2299" max="2299" width="5.28515625" style="3" customWidth="1"/>
-    <col min="2300" max="2300" width="6.85546875" style="3" customWidth="1"/>
+    <col min="2046" max="2046" width="30.6640625" style="3" customWidth="1"/>
+    <col min="2047" max="2048" width="9.109375" style="3" customWidth="1"/>
+    <col min="2049" max="2049" width="21.5546875" style="3" customWidth="1"/>
+    <col min="2050" max="2050" width="11.5546875" style="3" customWidth="1"/>
+    <col min="2051" max="2051" width="10.5546875" style="3" customWidth="1"/>
+    <col min="2052" max="2052" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2053" max="2297" width="8.88671875" style="3"/>
+    <col min="2298" max="2298" width="4.6640625" style="3" customWidth="1"/>
+    <col min="2299" max="2299" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2300" max="2300" width="6.88671875" style="3" customWidth="1"/>
     <col min="2301" max="2301" width="18" style="3" customWidth="1"/>
-    <col min="2302" max="2302" width="30.7109375" style="3" customWidth="1"/>
-    <col min="2303" max="2304" width="9.140625" style="3" customWidth="1"/>
-    <col min="2305" max="2305" width="21.5703125" style="3" customWidth="1"/>
-    <col min="2306" max="2306" width="11.5703125" style="3" customWidth="1"/>
-    <col min="2307" max="2307" width="10.5703125" style="3" customWidth="1"/>
-    <col min="2308" max="2308" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2309" max="2553" width="8.85546875" style="3"/>
-    <col min="2554" max="2554" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2555" max="2555" width="5.28515625" style="3" customWidth="1"/>
-    <col min="2556" max="2556" width="6.85546875" style="3" customWidth="1"/>
+    <col min="2302" max="2302" width="30.6640625" style="3" customWidth="1"/>
+    <col min="2303" max="2304" width="9.109375" style="3" customWidth="1"/>
+    <col min="2305" max="2305" width="21.5546875" style="3" customWidth="1"/>
+    <col min="2306" max="2306" width="11.5546875" style="3" customWidth="1"/>
+    <col min="2307" max="2307" width="10.5546875" style="3" customWidth="1"/>
+    <col min="2308" max="2308" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2309" max="2553" width="8.88671875" style="3"/>
+    <col min="2554" max="2554" width="4.6640625" style="3" customWidth="1"/>
+    <col min="2555" max="2555" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2556" max="2556" width="6.88671875" style="3" customWidth="1"/>
     <col min="2557" max="2557" width="18" style="3" customWidth="1"/>
-    <col min="2558" max="2558" width="30.7109375" style="3" customWidth="1"/>
-    <col min="2559" max="2560" width="9.140625" style="3" customWidth="1"/>
-    <col min="2561" max="2561" width="21.5703125" style="3" customWidth="1"/>
-    <col min="2562" max="2562" width="11.5703125" style="3" customWidth="1"/>
-    <col min="2563" max="2563" width="10.5703125" style="3" customWidth="1"/>
-    <col min="2564" max="2564" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2565" max="2809" width="8.85546875" style="3"/>
-    <col min="2810" max="2810" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2811" max="2811" width="5.28515625" style="3" customWidth="1"/>
-    <col min="2812" max="2812" width="6.85546875" style="3" customWidth="1"/>
+    <col min="2558" max="2558" width="30.6640625" style="3" customWidth="1"/>
+    <col min="2559" max="2560" width="9.109375" style="3" customWidth="1"/>
+    <col min="2561" max="2561" width="21.5546875" style="3" customWidth="1"/>
+    <col min="2562" max="2562" width="11.5546875" style="3" customWidth="1"/>
+    <col min="2563" max="2563" width="10.5546875" style="3" customWidth="1"/>
+    <col min="2564" max="2564" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2565" max="2809" width="8.88671875" style="3"/>
+    <col min="2810" max="2810" width="4.6640625" style="3" customWidth="1"/>
+    <col min="2811" max="2811" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2812" max="2812" width="6.88671875" style="3" customWidth="1"/>
     <col min="2813" max="2813" width="18" style="3" customWidth="1"/>
-    <col min="2814" max="2814" width="30.7109375" style="3" customWidth="1"/>
-    <col min="2815" max="2816" width="9.140625" style="3" customWidth="1"/>
-    <col min="2817" max="2817" width="21.5703125" style="3" customWidth="1"/>
-    <col min="2818" max="2818" width="11.5703125" style="3" customWidth="1"/>
-    <col min="2819" max="2819" width="10.5703125" style="3" customWidth="1"/>
-    <col min="2820" max="2820" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2821" max="3065" width="8.85546875" style="3"/>
-    <col min="3066" max="3066" width="4.7109375" style="3" customWidth="1"/>
-    <col min="3067" max="3067" width="5.28515625" style="3" customWidth="1"/>
-    <col min="3068" max="3068" width="6.85546875" style="3" customWidth="1"/>
+    <col min="2814" max="2814" width="30.6640625" style="3" customWidth="1"/>
+    <col min="2815" max="2816" width="9.109375" style="3" customWidth="1"/>
+    <col min="2817" max="2817" width="21.5546875" style="3" customWidth="1"/>
+    <col min="2818" max="2818" width="11.5546875" style="3" customWidth="1"/>
+    <col min="2819" max="2819" width="10.5546875" style="3" customWidth="1"/>
+    <col min="2820" max="2820" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2821" max="3065" width="8.88671875" style="3"/>
+    <col min="3066" max="3066" width="4.6640625" style="3" customWidth="1"/>
+    <col min="3067" max="3067" width="5.33203125" style="3" customWidth="1"/>
+    <col min="3068" max="3068" width="6.88671875" style="3" customWidth="1"/>
     <col min="3069" max="3069" width="18" style="3" customWidth="1"/>
-    <col min="3070" max="3070" width="30.7109375" style="3" customWidth="1"/>
-    <col min="3071" max="3072" width="9.140625" style="3" customWidth="1"/>
-    <col min="3073" max="3073" width="21.5703125" style="3" customWidth="1"/>
-    <col min="3074" max="3074" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3075" max="3075" width="10.5703125" style="3" customWidth="1"/>
-    <col min="3076" max="3076" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3077" max="3321" width="8.85546875" style="3"/>
-    <col min="3322" max="3322" width="4.7109375" style="3" customWidth="1"/>
-    <col min="3323" max="3323" width="5.28515625" style="3" customWidth="1"/>
-    <col min="3324" max="3324" width="6.85546875" style="3" customWidth="1"/>
+    <col min="3070" max="3070" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3071" max="3072" width="9.109375" style="3" customWidth="1"/>
+    <col min="3073" max="3073" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3074" max="3074" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3075" max="3075" width="10.5546875" style="3" customWidth="1"/>
+    <col min="3076" max="3076" width="12.33203125" style="3" customWidth="1"/>
+    <col min="3077" max="3321" width="8.88671875" style="3"/>
+    <col min="3322" max="3322" width="4.6640625" style="3" customWidth="1"/>
+    <col min="3323" max="3323" width="5.33203125" style="3" customWidth="1"/>
+    <col min="3324" max="3324" width="6.88671875" style="3" customWidth="1"/>
     <col min="3325" max="3325" width="18" style="3" customWidth="1"/>
-    <col min="3326" max="3326" width="30.7109375" style="3" customWidth="1"/>
-    <col min="3327" max="3328" width="9.140625" style="3" customWidth="1"/>
-    <col min="3329" max="3329" width="21.5703125" style="3" customWidth="1"/>
-    <col min="3330" max="3330" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3331" max="3331" width="10.5703125" style="3" customWidth="1"/>
-    <col min="3332" max="3332" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3333" max="3577" width="8.85546875" style="3"/>
-    <col min="3578" max="3578" width="4.7109375" style="3" customWidth="1"/>
-    <col min="3579" max="3579" width="5.28515625" style="3" customWidth="1"/>
-    <col min="3580" max="3580" width="6.85546875" style="3" customWidth="1"/>
+    <col min="3326" max="3326" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3327" max="3328" width="9.109375" style="3" customWidth="1"/>
+    <col min="3329" max="3329" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3330" max="3330" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3331" max="3331" width="10.5546875" style="3" customWidth="1"/>
+    <col min="3332" max="3332" width="12.33203125" style="3" customWidth="1"/>
+    <col min="3333" max="3577" width="8.88671875" style="3"/>
+    <col min="3578" max="3578" width="4.6640625" style="3" customWidth="1"/>
+    <col min="3579" max="3579" width="5.33203125" style="3" customWidth="1"/>
+    <col min="3580" max="3580" width="6.88671875" style="3" customWidth="1"/>
     <col min="3581" max="3581" width="18" style="3" customWidth="1"/>
-    <col min="3582" max="3582" width="30.7109375" style="3" customWidth="1"/>
-    <col min="3583" max="3584" width="9.140625" style="3" customWidth="1"/>
-    <col min="3585" max="3585" width="21.5703125" style="3" customWidth="1"/>
-    <col min="3586" max="3586" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3587" max="3587" width="10.5703125" style="3" customWidth="1"/>
-    <col min="3588" max="3588" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3589" max="3833" width="8.85546875" style="3"/>
-    <col min="3834" max="3834" width="4.7109375" style="3" customWidth="1"/>
-    <col min="3835" max="3835" width="5.28515625" style="3" customWidth="1"/>
-    <col min="3836" max="3836" width="6.85546875" style="3" customWidth="1"/>
+    <col min="3582" max="3582" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3583" max="3584" width="9.109375" style="3" customWidth="1"/>
+    <col min="3585" max="3585" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3586" max="3586" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3587" max="3587" width="10.5546875" style="3" customWidth="1"/>
+    <col min="3588" max="3588" width="12.33203125" style="3" customWidth="1"/>
+    <col min="3589" max="3833" width="8.88671875" style="3"/>
+    <col min="3834" max="3834" width="4.6640625" style="3" customWidth="1"/>
+    <col min="3835" max="3835" width="5.33203125" style="3" customWidth="1"/>
+    <col min="3836" max="3836" width="6.88671875" style="3" customWidth="1"/>
     <col min="3837" max="3837" width="18" style="3" customWidth="1"/>
-    <col min="3838" max="3838" width="30.7109375" style="3" customWidth="1"/>
-    <col min="3839" max="3840" width="9.140625" style="3" customWidth="1"/>
-    <col min="3841" max="3841" width="21.5703125" style="3" customWidth="1"/>
-    <col min="3842" max="3842" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3843" max="3843" width="10.5703125" style="3" customWidth="1"/>
-    <col min="3844" max="3844" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3845" max="4089" width="8.85546875" style="3"/>
-    <col min="4090" max="4090" width="4.7109375" style="3" customWidth="1"/>
-    <col min="4091" max="4091" width="5.28515625" style="3" customWidth="1"/>
-    <col min="4092" max="4092" width="6.85546875" style="3" customWidth="1"/>
+    <col min="3838" max="3838" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3839" max="3840" width="9.109375" style="3" customWidth="1"/>
+    <col min="3841" max="3841" width="21.5546875" style="3" customWidth="1"/>
+    <col min="3842" max="3842" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3843" max="3843" width="10.5546875" style="3" customWidth="1"/>
+    <col min="3844" max="3844" width="12.33203125" style="3" customWidth="1"/>
+    <col min="3845" max="4089" width="8.88671875" style="3"/>
+    <col min="4090" max="4090" width="4.6640625" style="3" customWidth="1"/>
+    <col min="4091" max="4091" width="5.33203125" style="3" customWidth="1"/>
+    <col min="4092" max="4092" width="6.88671875" style="3" customWidth="1"/>
     <col min="4093" max="4093" width="18" style="3" customWidth="1"/>
-    <col min="4094" max="4094" width="30.7109375" style="3" customWidth="1"/>
-    <col min="4095" max="4096" width="9.140625" style="3" customWidth="1"/>
-    <col min="4097" max="4097" width="21.5703125" style="3" customWidth="1"/>
-    <col min="4098" max="4098" width="11.5703125" style="3" customWidth="1"/>
-    <col min="4099" max="4099" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4100" max="4100" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4101" max="4345" width="8.85546875" style="3"/>
-    <col min="4346" max="4346" width="4.7109375" style="3" customWidth="1"/>
-    <col min="4347" max="4347" width="5.28515625" style="3" customWidth="1"/>
-    <col min="4348" max="4348" width="6.85546875" style="3" customWidth="1"/>
+    <col min="4094" max="4094" width="30.6640625" style="3" customWidth="1"/>
+    <col min="4095" max="4096" width="9.109375" style="3" customWidth="1"/>
+    <col min="4097" max="4097" width="21.5546875" style="3" customWidth="1"/>
+    <col min="4098" max="4098" width="11.5546875" style="3" customWidth="1"/>
+    <col min="4099" max="4099" width="10.5546875" style="3" customWidth="1"/>
+    <col min="4100" max="4100" width="12.33203125" style="3" customWidth="1"/>
+    <col min="4101" max="4345" width="8.88671875" style="3"/>
+    <col min="4346" max="4346" width="4.6640625" style="3" customWidth="1"/>
+    <col min="4347" max="4347" width="5.33203125" style="3" customWidth="1"/>
+    <col min="4348" max="4348" width="6.88671875" style="3" customWidth="1"/>
     <col min="4349" max="4349" width="18" style="3" customWidth="1"/>
-    <col min="4350" max="4350" width="30.7109375" style="3" customWidth="1"/>
-    <col min="4351" max="4352" width="9.140625" style="3" customWidth="1"/>
-    <col min="4353" max="4353" width="21.5703125" style="3" customWidth="1"/>
-    <col min="4354" max="4354" width="11.5703125" style="3" customWidth="1"/>
-    <col min="4355" max="4355" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4356" max="4356" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4357" max="4601" width="8.85546875" style="3"/>
-    <col min="4602" max="4602" width="4.7109375" style="3" customWidth="1"/>
-    <col min="4603" max="4603" width="5.28515625" style="3" customWidth="1"/>
-    <col min="4604" max="4604" width="6.85546875" style="3" customWidth="1"/>
+    <col min="4350" max="4350" width="30.6640625" style="3" customWidth="1"/>
+    <col min="4351" max="4352" width="9.109375" style="3" customWidth="1"/>
+    <col min="4353" max="4353" width="21.5546875" style="3" customWidth="1"/>
+    <col min="4354" max="4354" width="11.5546875" style="3" customWidth="1"/>
+    <col min="4355" max="4355" width="10.5546875" style="3" customWidth="1"/>
+    <col min="4356" max="4356" width="12.33203125" style="3" customWidth="1"/>
+    <col min="4357" max="4601" width="8.88671875" style="3"/>
+    <col min="4602" max="4602" width="4.6640625" style="3" customWidth="1"/>
+    <col min="4603" max="4603" width="5.33203125" style="3" customWidth="1"/>
+    <col min="4604" max="4604" width="6.88671875" style="3" customWidth="1"/>
     <col min="4605" max="4605" width="18" style="3" customWidth="1"/>
-    <col min="4606" max="4606" width="30.7109375" style="3" customWidth="1"/>
-    <col min="4607" max="4608" width="9.140625" style="3" customWidth="1"/>
-    <col min="4609" max="4609" width="21.5703125" style="3" customWidth="1"/>
-    <col min="4610" max="4610" width="11.5703125" style="3" customWidth="1"/>
-    <col min="4611" max="4611" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4612" max="4612" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4613" max="4857" width="8.85546875" style="3"/>
-    <col min="4858" max="4858" width="4.7109375" style="3" customWidth="1"/>
-    <col min="4859" max="4859" width="5.28515625" style="3" customWidth="1"/>
-    <col min="4860" max="4860" width="6.85546875" style="3" customWidth="1"/>
+    <col min="4606" max="4606" width="30.6640625" style="3" customWidth="1"/>
+    <col min="4607" max="4608" width="9.109375" style="3" customWidth="1"/>
+    <col min="4609" max="4609" width="21.5546875" style="3" customWidth="1"/>
+    <col min="4610" max="4610" width="11.5546875" style="3" customWidth="1"/>
+    <col min="4611" max="4611" width="10.5546875" style="3" customWidth="1"/>
+    <col min="4612" max="4612" width="12.33203125" style="3" customWidth="1"/>
+    <col min="4613" max="4857" width="8.88671875" style="3"/>
+    <col min="4858" max="4858" width="4.6640625" style="3" customWidth="1"/>
+    <col min="4859" max="4859" width="5.33203125" style="3" customWidth="1"/>
+    <col min="4860" max="4860" width="6.88671875" style="3" customWidth="1"/>
     <col min="4861" max="4861" width="18" style="3" customWidth="1"/>
-    <col min="4862" max="4862" width="30.7109375" style="3" customWidth="1"/>
-    <col min="4863" max="4864" width="9.140625" style="3" customWidth="1"/>
-    <col min="4865" max="4865" width="21.5703125" style="3" customWidth="1"/>
-    <col min="4866" max="4866" width="11.5703125" style="3" customWidth="1"/>
-    <col min="4867" max="4867" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4868" max="4868" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4869" max="5113" width="8.85546875" style="3"/>
-    <col min="5114" max="5114" width="4.7109375" style="3" customWidth="1"/>
-    <col min="5115" max="5115" width="5.28515625" style="3" customWidth="1"/>
-    <col min="5116" max="5116" width="6.85546875" style="3" customWidth="1"/>
+    <col min="4862" max="4862" width="30.6640625" style="3" customWidth="1"/>
+    <col min="4863" max="4864" width="9.109375" style="3" customWidth="1"/>
+    <col min="4865" max="4865" width="21.5546875" style="3" customWidth="1"/>
+    <col min="4866" max="4866" width="11.5546875" style="3" customWidth="1"/>
+    <col min="4867" max="4867" width="10.5546875" style="3" customWidth="1"/>
+    <col min="4868" max="4868" width="12.33203125" style="3" customWidth="1"/>
+    <col min="4869" max="5113" width="8.88671875" style="3"/>
+    <col min="5114" max="5114" width="4.6640625" style="3" customWidth="1"/>
+    <col min="5115" max="5115" width="5.33203125" style="3" customWidth="1"/>
+    <col min="5116" max="5116" width="6.88671875" style="3" customWidth="1"/>
     <col min="5117" max="5117" width="18" style="3" customWidth="1"/>
-    <col min="5118" max="5118" width="30.7109375" style="3" customWidth="1"/>
-    <col min="5119" max="5120" width="9.140625" style="3" customWidth="1"/>
-    <col min="5121" max="5121" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5122" max="5122" width="11.5703125" style="3" customWidth="1"/>
-    <col min="5123" max="5123" width="10.5703125" style="3" customWidth="1"/>
-    <col min="5124" max="5124" width="12.28515625" style="3" customWidth="1"/>
-    <col min="5125" max="5369" width="8.85546875" style="3"/>
-    <col min="5370" max="5370" width="4.7109375" style="3" customWidth="1"/>
-    <col min="5371" max="5371" width="5.28515625" style="3" customWidth="1"/>
-    <col min="5372" max="5372" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5118" max="5118" width="30.6640625" style="3" customWidth="1"/>
+    <col min="5119" max="5120" width="9.109375" style="3" customWidth="1"/>
+    <col min="5121" max="5121" width="21.5546875" style="3" customWidth="1"/>
+    <col min="5122" max="5122" width="11.5546875" style="3" customWidth="1"/>
+    <col min="5123" max="5123" width="10.5546875" style="3" customWidth="1"/>
+    <col min="5124" max="5124" width="12.33203125" style="3" customWidth="1"/>
+    <col min="5125" max="5369" width="8.88671875" style="3"/>
+    <col min="5370" max="5370" width="4.6640625" style="3" customWidth="1"/>
+    <col min="5371" max="5371" width="5.33203125" style="3" customWidth="1"/>
+    <col min="5372" max="5372" width="6.88671875" style="3" customWidth="1"/>
     <col min="5373" max="5373" width="18" style="3" customWidth="1"/>
-    <col min="5374" max="5374" width="30.7109375" style="3" customWidth="1"/>
-    <col min="5375" max="5376" width="9.140625" style="3" customWidth="1"/>
-    <col min="5377" max="5377" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5378" max="5378" width="11.5703125" style="3" customWidth="1"/>
-    <col min="5379" max="5379" width="10.5703125" style="3" customWidth="1"/>
-    <col min="5380" max="5380" width="12.28515625" style="3" customWidth="1"/>
-    <col min="5381" max="5625" width="8.85546875" style="3"/>
-    <col min="5626" max="5626" width="4.7109375" style="3" customWidth="1"/>
-    <col min="5627" max="5627" width="5.28515625" style="3" customWidth="1"/>
-    <col min="5628" max="5628" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5374" max="5374" width="30.6640625" style="3" customWidth="1"/>
+    <col min="5375" max="5376" width="9.109375" style="3" customWidth="1"/>
+    <col min="5377" max="5377" width="21.5546875" style="3" customWidth="1"/>
+    <col min="5378" max="5378" width="11.5546875" style="3" customWidth="1"/>
+    <col min="5379" max="5379" width="10.5546875" style="3" customWidth="1"/>
+    <col min="5380" max="5380" width="12.33203125" style="3" customWidth="1"/>
+    <col min="5381" max="5625" width="8.88671875" style="3"/>
+    <col min="5626" max="5626" width="4.6640625" style="3" customWidth="1"/>
+    <col min="5627" max="5627" width="5.33203125" style="3" customWidth="1"/>
+    <col min="5628" max="5628" width="6.88671875" style="3" customWidth="1"/>
     <col min="5629" max="5629" width="18" style="3" customWidth="1"/>
-    <col min="5630" max="5630" width="30.7109375" style="3" customWidth="1"/>
-    <col min="5631" max="5632" width="9.140625" style="3" customWidth="1"/>
-    <col min="5633" max="5633" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5634" max="5634" width="11.5703125" style="3" customWidth="1"/>
-    <col min="5635" max="5635" width="10.5703125" style="3" customWidth="1"/>
-    <col min="5636" max="5636" width="12.28515625" style="3" customWidth="1"/>
-    <col min="5637" max="5881" width="8.85546875" style="3"/>
-    <col min="5882" max="5882" width="4.7109375" style="3" customWidth="1"/>
-    <col min="5883" max="5883" width="5.28515625" style="3" customWidth="1"/>
-    <col min="5884" max="5884" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5630" max="5630" width="30.6640625" style="3" customWidth="1"/>
+    <col min="5631" max="5632" width="9.109375" style="3" customWidth="1"/>
+    <col min="5633" max="5633" width="21.5546875" style="3" customWidth="1"/>
+    <col min="5634" max="5634" width="11.5546875" style="3" customWidth="1"/>
+    <col min="5635" max="5635" width="10.5546875" style="3" customWidth="1"/>
+    <col min="5636" max="5636" width="12.33203125" style="3" customWidth="1"/>
+    <col min="5637" max="5881" width="8.88671875" style="3"/>
+    <col min="5882" max="5882" width="4.6640625" style="3" customWidth="1"/>
+    <col min="5883" max="5883" width="5.33203125" style="3" customWidth="1"/>
+    <col min="5884" max="5884" width="6.88671875" style="3" customWidth="1"/>
     <col min="5885" max="5885" width="18" style="3" customWidth="1"/>
-    <col min="5886" max="5886" width="30.7109375" style="3" customWidth="1"/>
-    <col min="5887" max="5888" width="9.140625" style="3" customWidth="1"/>
-    <col min="5889" max="5889" width="21.5703125" style="3" customWidth="1"/>
-    <col min="5890" max="5890" width="11.5703125" style="3" customWidth="1"/>
-    <col min="5891" max="5891" width="10.5703125" style="3" customWidth="1"/>
-    <col min="5892" max="5892" width="12.28515625" style="3" customWidth="1"/>
-    <col min="5893" max="6137" width="8.85546875" style="3"/>
-    <col min="6138" max="6138" width="4.7109375" style="3" customWidth="1"/>
-    <col min="6139" max="6139" width="5.28515625" style="3" customWidth="1"/>
-    <col min="6140" max="6140" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5886" max="5886" width="30.6640625" style="3" customWidth="1"/>
+    <col min="5887" max="5888" width="9.109375" style="3" customWidth="1"/>
+    <col min="5889" max="5889" width="21.5546875" style="3" customWidth="1"/>
+    <col min="5890" max="5890" width="11.5546875" style="3" customWidth="1"/>
+    <col min="5891" max="5891" width="10.5546875" style="3" customWidth="1"/>
+    <col min="5892" max="5892" width="12.33203125" style="3" customWidth="1"/>
+    <col min="5893" max="6137" width="8.88671875" style="3"/>
+    <col min="6138" max="6138" width="4.6640625" style="3" customWidth="1"/>
+    <col min="6139" max="6139" width="5.33203125" style="3" customWidth="1"/>
+    <col min="6140" max="6140" width="6.88671875" style="3" customWidth="1"/>
     <col min="6141" max="6141" width="18" style="3" customWidth="1"/>
-    <col min="6142" max="6142" width="30.7109375" style="3" customWidth="1"/>
-    <col min="6143" max="6144" width="9.140625" style="3" customWidth="1"/>
-    <col min="6145" max="6145" width="21.5703125" style="3" customWidth="1"/>
-    <col min="6146" max="6146" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6147" max="6147" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6148" max="6148" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6149" max="6393" width="8.85546875" style="3"/>
-    <col min="6394" max="6394" width="4.7109375" style="3" customWidth="1"/>
-    <col min="6395" max="6395" width="5.28515625" style="3" customWidth="1"/>
-    <col min="6396" max="6396" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6142" max="6142" width="30.6640625" style="3" customWidth="1"/>
+    <col min="6143" max="6144" width="9.109375" style="3" customWidth="1"/>
+    <col min="6145" max="6145" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6146" max="6146" width="11.5546875" style="3" customWidth="1"/>
+    <col min="6147" max="6147" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6148" max="6148" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6149" max="6393" width="8.88671875" style="3"/>
+    <col min="6394" max="6394" width="4.6640625" style="3" customWidth="1"/>
+    <col min="6395" max="6395" width="5.33203125" style="3" customWidth="1"/>
+    <col min="6396" max="6396" width="6.88671875" style="3" customWidth="1"/>
     <col min="6397" max="6397" width="18" style="3" customWidth="1"/>
-    <col min="6398" max="6398" width="30.7109375" style="3" customWidth="1"/>
-    <col min="6399" max="6400" width="9.140625" style="3" customWidth="1"/>
-    <col min="6401" max="6401" width="21.5703125" style="3" customWidth="1"/>
-    <col min="6402" max="6402" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6403" max="6403" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6404" max="6404" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6405" max="6649" width="8.85546875" style="3"/>
-    <col min="6650" max="6650" width="4.7109375" style="3" customWidth="1"/>
-    <col min="6651" max="6651" width="5.28515625" style="3" customWidth="1"/>
-    <col min="6652" max="6652" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6398" max="6398" width="30.6640625" style="3" customWidth="1"/>
+    <col min="6399" max="6400" width="9.109375" style="3" customWidth="1"/>
+    <col min="6401" max="6401" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6402" max="6402" width="11.5546875" style="3" customWidth="1"/>
+    <col min="6403" max="6403" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6404" max="6404" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6405" max="6649" width="8.88671875" style="3"/>
+    <col min="6650" max="6650" width="4.6640625" style="3" customWidth="1"/>
+    <col min="6651" max="6651" width="5.33203125" style="3" customWidth="1"/>
+    <col min="6652" max="6652" width="6.88671875" style="3" customWidth="1"/>
     <col min="6653" max="6653" width="18" style="3" customWidth="1"/>
-    <col min="6654" max="6654" width="30.7109375" style="3" customWidth="1"/>
-    <col min="6655" max="6656" width="9.140625" style="3" customWidth="1"/>
-    <col min="6657" max="6657" width="21.5703125" style="3" customWidth="1"/>
-    <col min="6658" max="6658" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6659" max="6659" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6660" max="6660" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6661" max="6905" width="8.85546875" style="3"/>
-    <col min="6906" max="6906" width="4.7109375" style="3" customWidth="1"/>
-    <col min="6907" max="6907" width="5.28515625" style="3" customWidth="1"/>
-    <col min="6908" max="6908" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6654" max="6654" width="30.6640625" style="3" customWidth="1"/>
+    <col min="6655" max="6656" width="9.109375" style="3" customWidth="1"/>
+    <col min="6657" max="6657" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6658" max="6658" width="11.5546875" style="3" customWidth="1"/>
+    <col min="6659" max="6659" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6660" max="6660" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6661" max="6905" width="8.88671875" style="3"/>
+    <col min="6906" max="6906" width="4.6640625" style="3" customWidth="1"/>
+    <col min="6907" max="6907" width="5.33203125" style="3" customWidth="1"/>
+    <col min="6908" max="6908" width="6.88671875" style="3" customWidth="1"/>
     <col min="6909" max="6909" width="18" style="3" customWidth="1"/>
-    <col min="6910" max="6910" width="30.7109375" style="3" customWidth="1"/>
-    <col min="6911" max="6912" width="9.140625" style="3" customWidth="1"/>
-    <col min="6913" max="6913" width="21.5703125" style="3" customWidth="1"/>
-    <col min="6914" max="6914" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6915" max="6915" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6916" max="6916" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6917" max="7161" width="8.85546875" style="3"/>
-    <col min="7162" max="7162" width="4.7109375" style="3" customWidth="1"/>
-    <col min="7163" max="7163" width="5.28515625" style="3" customWidth="1"/>
-    <col min="7164" max="7164" width="6.85546875" style="3" customWidth="1"/>
+    <col min="6910" max="6910" width="30.6640625" style="3" customWidth="1"/>
+    <col min="6911" max="6912" width="9.109375" style="3" customWidth="1"/>
+    <col min="6913" max="6913" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6914" max="6914" width="11.5546875" style="3" customWidth="1"/>
+    <col min="6915" max="6915" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6916" max="6916" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6917" max="7161" width="8.88671875" style="3"/>
+    <col min="7162" max="7162" width="4.6640625" style="3" customWidth="1"/>
+    <col min="7163" max="7163" width="5.33203125" style="3" customWidth="1"/>
+    <col min="7164" max="7164" width="6.88671875" style="3" customWidth="1"/>
     <col min="7165" max="7165" width="18" style="3" customWidth="1"/>
-    <col min="7166" max="7166" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7167" max="7168" width="9.140625" style="3" customWidth="1"/>
-    <col min="7169" max="7169" width="21.5703125" style="3" customWidth="1"/>
-    <col min="7170" max="7170" width="11.5703125" style="3" customWidth="1"/>
-    <col min="7171" max="7171" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7172" max="7172" width="12.28515625" style="3" customWidth="1"/>
-    <col min="7173" max="7417" width="8.85546875" style="3"/>
-    <col min="7418" max="7418" width="4.7109375" style="3" customWidth="1"/>
-    <col min="7419" max="7419" width="5.28515625" style="3" customWidth="1"/>
-    <col min="7420" max="7420" width="6.85546875" style="3" customWidth="1"/>
+    <col min="7166" max="7166" width="30.6640625" style="3" customWidth="1"/>
+    <col min="7167" max="7168" width="9.109375" style="3" customWidth="1"/>
+    <col min="7169" max="7169" width="21.5546875" style="3" customWidth="1"/>
+    <col min="7170" max="7170" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7171" max="7171" width="10.5546875" style="3" customWidth="1"/>
+    <col min="7172" max="7172" width="12.33203125" style="3" customWidth="1"/>
+    <col min="7173" max="7417" width="8.88671875" style="3"/>
+    <col min="7418" max="7418" width="4.6640625" style="3" customWidth="1"/>
+    <col min="7419" max="7419" width="5.33203125" style="3" customWidth="1"/>
+    <col min="7420" max="7420" width="6.88671875" style="3" customWidth="1"/>
     <col min="7421" max="7421" width="18" style="3" customWidth="1"/>
-    <col min="7422" max="7422" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7423" max="7424" width="9.140625" style="3" customWidth="1"/>
-    <col min="7425" max="7425" width="21.5703125" style="3" customWidth="1"/>
-    <col min="7426" max="7426" width="11.5703125" style="3" customWidth="1"/>
-    <col min="7427" max="7427" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7428" max="7428" width="12.28515625" style="3" customWidth="1"/>
-    <col min="7429" max="7673" width="8.85546875" style="3"/>
-    <col min="7674" max="7674" width="4.7109375" style="3" customWidth="1"/>
-    <col min="7675" max="7675" width="5.28515625" style="3" customWidth="1"/>
-    <col min="7676" max="7676" width="6.85546875" style="3" customWidth="1"/>
+    <col min="7422" max="7422" width="30.6640625" style="3" customWidth="1"/>
+    <col min="7423" max="7424" width="9.109375" style="3" customWidth="1"/>
+    <col min="7425" max="7425" width="21.5546875" style="3" customWidth="1"/>
+    <col min="7426" max="7426" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7427" max="7427" width="10.5546875" style="3" customWidth="1"/>
+    <col min="7428" max="7428" width="12.33203125" style="3" customWidth="1"/>
+    <col min="7429" max="7673" width="8.88671875" style="3"/>
+    <col min="7674" max="7674" width="4.6640625" style="3" customWidth="1"/>
+    <col min="7675" max="7675" width="5.33203125" style="3" customWidth="1"/>
+    <col min="7676" max="7676" width="6.88671875" style="3" customWidth="1"/>
     <col min="7677" max="7677" width="18" style="3" customWidth="1"/>
-    <col min="7678" max="7678" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7679" max="7680" width="9.140625" style="3" customWidth="1"/>
-    <col min="7681" max="7681" width="21.5703125" style="3" customWidth="1"/>
-    <col min="7682" max="7682" width="11.5703125" style="3" customWidth="1"/>
-    <col min="7683" max="7683" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7684" max="7684" width="12.28515625" style="3" customWidth="1"/>
-    <col min="7685" max="7929" width="8.85546875" style="3"/>
-    <col min="7930" max="7930" width="4.7109375" style="3" customWidth="1"/>
-    <col min="7931" max="7931" width="5.28515625" style="3" customWidth="1"/>
-    <col min="7932" max="7932" width="6.85546875" style="3" customWidth="1"/>
+    <col min="7678" max="7678" width="30.6640625" style="3" customWidth="1"/>
+    <col min="7679" max="7680" width="9.109375" style="3" customWidth="1"/>
+    <col min="7681" max="7681" width="21.5546875" style="3" customWidth="1"/>
+    <col min="7682" max="7682" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7683" max="7683" width="10.5546875" style="3" customWidth="1"/>
+    <col min="7684" max="7684" width="12.33203125" style="3" customWidth="1"/>
+    <col min="7685" max="7929" width="8.88671875" style="3"/>
+    <col min="7930" max="7930" width="4.6640625" style="3" customWidth="1"/>
+    <col min="7931" max="7931" width="5.33203125" style="3" customWidth="1"/>
+    <col min="7932" max="7932" width="6.88671875" style="3" customWidth="1"/>
     <col min="7933" max="7933" width="18" style="3" customWidth="1"/>
-    <col min="7934" max="7934" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7935" max="7936" width="9.140625" style="3" customWidth="1"/>
-    <col min="7937" max="7937" width="21.5703125" style="3" customWidth="1"/>
-    <col min="7938" max="7938" width="11.5703125" style="3" customWidth="1"/>
-    <col min="7939" max="7939" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7940" max="7940" width="12.28515625" style="3" customWidth="1"/>
-    <col min="7941" max="8185" width="8.85546875" style="3"/>
-    <col min="8186" max="8186" width="4.7109375" style="3" customWidth="1"/>
-    <col min="8187" max="8187" width="5.28515625" style="3" customWidth="1"/>
-    <col min="8188" max="8188" width="6.85546875" style="3" customWidth="1"/>
+    <col min="7934" max="7934" width="30.6640625" style="3" customWidth="1"/>
+    <col min="7935" max="7936" width="9.109375" style="3" customWidth="1"/>
+    <col min="7937" max="7937" width="21.5546875" style="3" customWidth="1"/>
+    <col min="7938" max="7938" width="11.5546875" style="3" customWidth="1"/>
+    <col min="7939" max="7939" width="10.5546875" style="3" customWidth="1"/>
+    <col min="7940" max="7940" width="12.33203125" style="3" customWidth="1"/>
+    <col min="7941" max="8185" width="8.88671875" style="3"/>
+    <col min="8186" max="8186" width="4.6640625" style="3" customWidth="1"/>
+    <col min="8187" max="8187" width="5.33203125" style="3" customWidth="1"/>
+    <col min="8188" max="8188" width="6.88671875" style="3" customWidth="1"/>
     <col min="8189" max="8189" width="18" style="3" customWidth="1"/>
-    <col min="8190" max="8190" width="30.7109375" style="3" customWidth="1"/>
-    <col min="8191" max="8192" width="9.140625" style="3" customWidth="1"/>
-    <col min="8193" max="8193" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8194" max="8194" width="11.5703125" style="3" customWidth="1"/>
-    <col min="8195" max="8195" width="10.5703125" style="3" customWidth="1"/>
-    <col min="8196" max="8196" width="12.28515625" style="3" customWidth="1"/>
-    <col min="8197" max="8441" width="8.85546875" style="3"/>
-    <col min="8442" max="8442" width="4.7109375" style="3" customWidth="1"/>
-    <col min="8443" max="8443" width="5.28515625" style="3" customWidth="1"/>
-    <col min="8444" max="8444" width="6.85546875" style="3" customWidth="1"/>
+    <col min="8190" max="8190" width="30.6640625" style="3" customWidth="1"/>
+    <col min="8191" max="8192" width="9.109375" style="3" customWidth="1"/>
+    <col min="8193" max="8193" width="21.5546875" style="3" customWidth="1"/>
+    <col min="8194" max="8194" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8195" max="8195" width="10.5546875" style="3" customWidth="1"/>
+    <col min="8196" max="8196" width="12.33203125" style="3" customWidth="1"/>
+    <col min="8197" max="8441" width="8.88671875" style="3"/>
+    <col min="8442" max="8442" width="4.6640625" style="3" customWidth="1"/>
+    <col min="8443" max="8443" width="5.33203125" style="3" customWidth="1"/>
+    <col min="8444" max="8444" width="6.88671875" style="3" customWidth="1"/>
     <col min="8445" max="8445" width="18" style="3" customWidth="1"/>
-    <col min="8446" max="8446" width="30.7109375" style="3" customWidth="1"/>
-    <col min="8447" max="8448" width="9.140625" style="3" customWidth="1"/>
-    <col min="8449" max="8449" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8450" max="8450" width="11.5703125" style="3" customWidth="1"/>
-    <col min="8451" max="8451" width="10.5703125" style="3" customWidth="1"/>
-    <col min="8452" max="8452" width="12.28515625" style="3" customWidth="1"/>
-    <col min="8453" max="8697" width="8.85546875" style="3"/>
-    <col min="8698" max="8698" width="4.7109375" style="3" customWidth="1"/>
-    <col min="8699" max="8699" width="5.28515625" style="3" customWidth="1"/>
-    <col min="8700" max="8700" width="6.85546875" style="3" customWidth="1"/>
+    <col min="8446" max="8446" width="30.6640625" style="3" customWidth="1"/>
+    <col min="8447" max="8448" width="9.109375" style="3" customWidth="1"/>
+    <col min="8449" max="8449" width="21.5546875" style="3" customWidth="1"/>
+    <col min="8450" max="8450" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8451" max="8451" width="10.5546875" style="3" customWidth="1"/>
+    <col min="8452" max="8452" width="12.33203125" style="3" customWidth="1"/>
+    <col min="8453" max="8697" width="8.88671875" style="3"/>
+    <col min="8698" max="8698" width="4.6640625" style="3" customWidth="1"/>
+    <col min="8699" max="8699" width="5.33203125" style="3" customWidth="1"/>
+    <col min="8700" max="8700" width="6.88671875" style="3" customWidth="1"/>
     <col min="8701" max="8701" width="18" style="3" customWidth="1"/>
-    <col min="8702" max="8702" width="30.7109375" style="3" customWidth="1"/>
-    <col min="8703" max="8704" width="9.140625" style="3" customWidth="1"/>
-    <col min="8705" max="8705" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8706" max="8706" width="11.5703125" style="3" customWidth="1"/>
-    <col min="8707" max="8707" width="10.5703125" style="3" customWidth="1"/>
-    <col min="8708" max="8708" width="12.28515625" style="3" customWidth="1"/>
-    <col min="8709" max="8953" width="8.85546875" style="3"/>
-    <col min="8954" max="8954" width="4.7109375" style="3" customWidth="1"/>
-    <col min="8955" max="8955" width="5.28515625" style="3" customWidth="1"/>
-    <col min="8956" max="8956" width="6.85546875" style="3" customWidth="1"/>
+    <col min="8702" max="8702" width="30.6640625" style="3" customWidth="1"/>
+    <col min="8703" max="8704" width="9.109375" style="3" customWidth="1"/>
+    <col min="8705" max="8705" width="21.5546875" style="3" customWidth="1"/>
+    <col min="8706" max="8706" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8707" max="8707" width="10.5546875" style="3" customWidth="1"/>
+    <col min="8708" max="8708" width="12.33203125" style="3" customWidth="1"/>
+    <col min="8709" max="8953" width="8.88671875" style="3"/>
+    <col min="8954" max="8954" width="4.6640625" style="3" customWidth="1"/>
+    <col min="8955" max="8955" width="5.33203125" style="3" customWidth="1"/>
+    <col min="8956" max="8956" width="6.88671875" style="3" customWidth="1"/>
     <col min="8957" max="8957" width="18" style="3" customWidth="1"/>
-    <col min="8958" max="8958" width="30.7109375" style="3" customWidth="1"/>
-    <col min="8959" max="8960" width="9.140625" style="3" customWidth="1"/>
-    <col min="8961" max="8961" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8962" max="8962" width="11.5703125" style="3" customWidth="1"/>
-    <col min="8963" max="8963" width="10.5703125" style="3" customWidth="1"/>
-    <col min="8964" max="8964" width="12.28515625" style="3" customWidth="1"/>
-    <col min="8965" max="9209" width="8.85546875" style="3"/>
-    <col min="9210" max="9210" width="4.7109375" style="3" customWidth="1"/>
-    <col min="9211" max="9211" width="5.28515625" style="3" customWidth="1"/>
-    <col min="9212" max="9212" width="6.85546875" style="3" customWidth="1"/>
+    <col min="8958" max="8958" width="30.6640625" style="3" customWidth="1"/>
+    <col min="8959" max="8960" width="9.109375" style="3" customWidth="1"/>
+    <col min="8961" max="8961" width="21.5546875" style="3" customWidth="1"/>
+    <col min="8962" max="8962" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8963" max="8963" width="10.5546875" style="3" customWidth="1"/>
+    <col min="8964" max="8964" width="12.33203125" style="3" customWidth="1"/>
+    <col min="8965" max="9209" width="8.88671875" style="3"/>
+    <col min="9210" max="9210" width="4.6640625" style="3" customWidth="1"/>
+    <col min="9211" max="9211" width="5.33203125" style="3" customWidth="1"/>
+    <col min="9212" max="9212" width="6.88671875" style="3" customWidth="1"/>
     <col min="9213" max="9213" width="18" style="3" customWidth="1"/>
-    <col min="9214" max="9214" width="30.7109375" style="3" customWidth="1"/>
-    <col min="9215" max="9216" width="9.140625" style="3" customWidth="1"/>
-    <col min="9217" max="9217" width="21.5703125" style="3" customWidth="1"/>
-    <col min="9218" max="9218" width="11.5703125" style="3" customWidth="1"/>
-    <col min="9219" max="9219" width="10.5703125" style="3" customWidth="1"/>
-    <col min="9220" max="9220" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9221" max="9465" width="8.85546875" style="3"/>
-    <col min="9466" max="9466" width="4.7109375" style="3" customWidth="1"/>
-    <col min="9467" max="9467" width="5.28515625" style="3" customWidth="1"/>
-    <col min="9468" max="9468" width="6.85546875" style="3" customWidth="1"/>
+    <col min="9214" max="9214" width="30.6640625" style="3" customWidth="1"/>
+    <col min="9215" max="9216" width="9.109375" style="3" customWidth="1"/>
+    <col min="9217" max="9217" width="21.5546875" style="3" customWidth="1"/>
+    <col min="9218" max="9218" width="11.5546875" style="3" customWidth="1"/>
+    <col min="9219" max="9219" width="10.5546875" style="3" customWidth="1"/>
+    <col min="9220" max="9220" width="12.33203125" style="3" customWidth="1"/>
+    <col min="9221" max="9465" width="8.88671875" style="3"/>
+    <col min="9466" max="9466" width="4.6640625" style="3" customWidth="1"/>
+    <col min="9467" max="9467" width="5.33203125" style="3" customWidth="1"/>
+    <col min="9468" max="9468" width="6.88671875" style="3" customWidth="1"/>
     <col min="9469" max="9469" width="18" style="3" customWidth="1"/>
-    <col min="9470" max="9470" width="30.7109375" style="3" customWidth="1"/>
-    <col min="9471" max="9472" width="9.140625" style="3" customWidth="1"/>
-    <col min="9473" max="9473" width="21.5703125" style="3" customWidth="1"/>
-    <col min="9474" max="9474" width="11.5703125" style="3" customWidth="1"/>
-    <col min="9475" max="9475" width="10.5703125" style="3" customWidth="1"/>
-    <col min="9476" max="9476" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9477" max="9721" width="8.85546875" style="3"/>
-    <col min="9722" max="9722" width="4.7109375" style="3" customWidth="1"/>
-    <col min="9723" max="9723" width="5.28515625" style="3" customWidth="1"/>
-    <col min="9724" max="9724" width="6.85546875" style="3" customWidth="1"/>
+    <col min="9470" max="9470" width="30.6640625" style="3" customWidth="1"/>
+    <col min="9471" max="9472" width="9.109375" style="3" customWidth="1"/>
+    <col min="9473" max="9473" width="21.5546875" style="3" customWidth="1"/>
+    <col min="9474" max="9474" width="11.5546875" style="3" customWidth="1"/>
+    <col min="9475" max="9475" width="10.5546875" style="3" customWidth="1"/>
+    <col min="9476" max="9476" width="12.33203125" style="3" customWidth="1"/>
+    <col min="9477" max="9721" width="8.88671875" style="3"/>
+    <col min="9722" max="9722" width="4.6640625" style="3" customWidth="1"/>
+    <col min="9723" max="9723" width="5.33203125" style="3" customWidth="1"/>
+    <col min="9724" max="9724" width="6.88671875" style="3" customWidth="1"/>
     <col min="9725" max="9725" width="18" style="3" customWidth="1"/>
-    <col min="9726" max="9726" width="30.7109375" style="3" customWidth="1"/>
-    <col min="9727" max="9728" width="9.140625" style="3" customWidth="1"/>
-    <col min="9729" max="9729" width="21.5703125" style="3" customWidth="1"/>
-    <col min="9730" max="9730" width="11.5703125" style="3" customWidth="1"/>
-    <col min="9731" max="9731" width="10.5703125" style="3" customWidth="1"/>
-    <col min="9732" max="9732" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9733" max="9977" width="8.85546875" style="3"/>
-    <col min="9978" max="9978" width="4.7109375" style="3" customWidth="1"/>
-    <col min="9979" max="9979" width="5.28515625" style="3" customWidth="1"/>
-    <col min="9980" max="9980" width="6.85546875" style="3" customWidth="1"/>
+    <col min="9726" max="9726" width="30.6640625" style="3" customWidth="1"/>
+    <col min="9727" max="9728" width="9.109375" style="3" customWidth="1"/>
+    <col min="9729" max="9729" width="21.5546875" style="3" customWidth="1"/>
+    <col min="9730" max="9730" width="11.5546875" style="3" customWidth="1"/>
+    <col min="9731" max="9731" width="10.5546875" style="3" customWidth="1"/>
+    <col min="9732" max="9732" width="12.33203125" style="3" customWidth="1"/>
+    <col min="9733" max="9977" width="8.88671875" style="3"/>
+    <col min="9978" max="9978" width="4.6640625" style="3" customWidth="1"/>
+    <col min="9979" max="9979" width="5.33203125" style="3" customWidth="1"/>
+    <col min="9980" max="9980" width="6.88671875" style="3" customWidth="1"/>
     <col min="9981" max="9981" width="18" style="3" customWidth="1"/>
-    <col min="9982" max="9982" width="30.7109375" style="3" customWidth="1"/>
-    <col min="9983" max="9984" width="9.140625" style="3" customWidth="1"/>
-    <col min="9985" max="9985" width="21.5703125" style="3" customWidth="1"/>
-    <col min="9986" max="9986" width="11.5703125" style="3" customWidth="1"/>
-    <col min="9987" max="9987" width="10.5703125" style="3" customWidth="1"/>
-    <col min="9988" max="9988" width="12.28515625" style="3" customWidth="1"/>
-    <col min="9989" max="10233" width="8.85546875" style="3"/>
-    <col min="10234" max="10234" width="4.7109375" style="3" customWidth="1"/>
-    <col min="10235" max="10235" width="5.28515625" style="3" customWidth="1"/>
-    <col min="10236" max="10236" width="6.85546875" style="3" customWidth="1"/>
+    <col min="9982" max="9982" width="30.6640625" style="3" customWidth="1"/>
+    <col min="9983" max="9984" width="9.109375" style="3" customWidth="1"/>
+    <col min="9985" max="9985" width="21.5546875" style="3" customWidth="1"/>
+    <col min="9986" max="9986" width="11.5546875" style="3" customWidth="1"/>
+    <col min="9987" max="9987" width="10.5546875" style="3" customWidth="1"/>
+    <col min="9988" max="9988" width="12.33203125" style="3" customWidth="1"/>
+    <col min="9989" max="10233" width="8.88671875" style="3"/>
+    <col min="10234" max="10234" width="4.6640625" style="3" customWidth="1"/>
+    <col min="10235" max="10235" width="5.33203125" style="3" customWidth="1"/>
+    <col min="10236" max="10236" width="6.88671875" style="3" customWidth="1"/>
     <col min="10237" max="10237" width="18" style="3" customWidth="1"/>
-    <col min="10238" max="10238" width="30.7109375" style="3" customWidth="1"/>
-    <col min="10239" max="10240" width="9.140625" style="3" customWidth="1"/>
-    <col min="10241" max="10241" width="21.5703125" style="3" customWidth="1"/>
-    <col min="10242" max="10242" width="11.5703125" style="3" customWidth="1"/>
-    <col min="10243" max="10243" width="10.5703125" style="3" customWidth="1"/>
-    <col min="10244" max="10244" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10245" max="10489" width="8.85546875" style="3"/>
-    <col min="10490" max="10490" width="4.7109375" style="3" customWidth="1"/>
-    <col min="10491" max="10491" width="5.28515625" style="3" customWidth="1"/>
-    <col min="10492" max="10492" width="6.85546875" style="3" customWidth="1"/>
+    <col min="10238" max="10238" width="30.6640625" style="3" customWidth="1"/>
+    <col min="10239" max="10240" width="9.109375" style="3" customWidth="1"/>
+    <col min="10241" max="10241" width="21.5546875" style="3" customWidth="1"/>
+    <col min="10242" max="10242" width="11.5546875" style="3" customWidth="1"/>
+    <col min="10243" max="10243" width="10.5546875" style="3" customWidth="1"/>
+    <col min="10244" max="10244" width="12.33203125" style="3" customWidth="1"/>
+    <col min="10245" max="10489" width="8.88671875" style="3"/>
+    <col min="10490" max="10490" width="4.6640625" style="3" customWidth="1"/>
+    <col min="10491" max="10491" width="5.33203125" style="3" customWidth="1"/>
+    <col min="10492" max="10492" width="6.88671875" style="3" customWidth="1"/>
     <col min="10493" max="10493" width="18" style="3" customWidth="1"/>
-    <col min="10494" max="10494" width="30.7109375" style="3" customWidth="1"/>
-    <col min="10495" max="10496" width="9.140625" style="3" customWidth="1"/>
-    <col min="10497" max="10497" width="21.5703125" style="3" customWidth="1"/>
-    <col min="10498" max="10498" width="11.5703125" style="3" customWidth="1"/>
-    <col min="10499" max="10499" width="10.5703125" style="3" customWidth="1"/>
-    <col min="10500" max="10500" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10501" max="10745" width="8.85546875" style="3"/>
-    <col min="10746" max="10746" width="4.7109375" style="3" customWidth="1"/>
-    <col min="10747" max="10747" width="5.28515625" style="3" customWidth="1"/>
-    <col min="10748" max="10748" width="6.85546875" style="3" customWidth="1"/>
+    <col min="10494" max="10494" width="30.6640625" style="3" customWidth="1"/>
+    <col min="10495" max="10496" width="9.109375" style="3" customWidth="1"/>
+    <col min="10497" max="10497" width="21.5546875" style="3" customWidth="1"/>
+    <col min="10498" max="10498" width="11.5546875" style="3" customWidth="1"/>
+    <col min="10499" max="10499" width="10.5546875" style="3" customWidth="1"/>
+    <col min="10500" max="10500" width="12.33203125" style="3" customWidth="1"/>
+    <col min="10501" max="10745" width="8.88671875" style="3"/>
+    <col min="10746" max="10746" width="4.6640625" style="3" customWidth="1"/>
+    <col min="10747" max="10747" width="5.33203125" style="3" customWidth="1"/>
+    <col min="10748" max="10748" width="6.88671875" style="3" customWidth="1"/>
     <col min="10749" max="10749" width="18" style="3" customWidth="1"/>
-    <col min="10750" max="10750" width="30.7109375" style="3" customWidth="1"/>
-    <col min="10751" max="10752" width="9.140625" style="3" customWidth="1"/>
-    <col min="10753" max="10753" width="21.5703125" style="3" customWidth="1"/>
-    <col min="10754" max="10754" width="11.5703125" style="3" customWidth="1"/>
-    <col min="10755" max="10755" width="10.5703125" style="3" customWidth="1"/>
-    <col min="10756" max="10756" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10757" max="11001" width="8.85546875" style="3"/>
-    <col min="11002" max="11002" width="4.7109375" style="3" customWidth="1"/>
-    <col min="11003" max="11003" width="5.28515625" style="3" customWidth="1"/>
-    <col min="11004" max="11004" width="6.85546875" style="3" customWidth="1"/>
+    <col min="10750" max="10750" width="30.6640625" style="3" customWidth="1"/>
+    <col min="10751" max="10752" width="9.109375" style="3" customWidth="1"/>
+    <col min="10753" max="10753" width="21.5546875" style="3" customWidth="1"/>
+    <col min="10754" max="10754" width="11.5546875" style="3" customWidth="1"/>
+    <col min="10755" max="10755" width="10.5546875" style="3" customWidth="1"/>
+    <col min="10756" max="10756" width="12.33203125" style="3" customWidth="1"/>
+    <col min="10757" max="11001" width="8.88671875" style="3"/>
+    <col min="11002" max="11002" width="4.6640625" style="3" customWidth="1"/>
+    <col min="11003" max="11003" width="5.33203125" style="3" customWidth="1"/>
+    <col min="11004" max="11004" width="6.88671875" style="3" customWidth="1"/>
     <col min="11005" max="11005" width="18" style="3" customWidth="1"/>
-    <col min="11006" max="11006" width="30.7109375" style="3" customWidth="1"/>
-    <col min="11007" max="11008" width="9.140625" style="3" customWidth="1"/>
-    <col min="11009" max="11009" width="21.5703125" style="3" customWidth="1"/>
-    <col min="11010" max="11010" width="11.5703125" style="3" customWidth="1"/>
-    <col min="11011" max="11011" width="10.5703125" style="3" customWidth="1"/>
-    <col min="11012" max="11012" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11013" max="11257" width="8.85546875" style="3"/>
-    <col min="11258" max="11258" width="4.7109375" style="3" customWidth="1"/>
-    <col min="11259" max="11259" width="5.28515625" style="3" customWidth="1"/>
-    <col min="11260" max="11260" width="6.85546875" style="3" customWidth="1"/>
+    <col min="11006" max="11006" width="30.6640625" style="3" customWidth="1"/>
+    <col min="11007" max="11008" width="9.109375" style="3" customWidth="1"/>
+    <col min="11009" max="11009" width="21.5546875" style="3" customWidth="1"/>
+    <col min="11010" max="11010" width="11.5546875" style="3" customWidth="1"/>
+    <col min="11011" max="11011" width="10.5546875" style="3" customWidth="1"/>
+    <col min="11012" max="11012" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11013" max="11257" width="8.88671875" style="3"/>
+    <col min="11258" max="11258" width="4.6640625" style="3" customWidth="1"/>
+    <col min="11259" max="11259" width="5.33203125" style="3" customWidth="1"/>
+    <col min="11260" max="11260" width="6.88671875" style="3" customWidth="1"/>
     <col min="11261" max="11261" width="18" style="3" customWidth="1"/>
-    <col min="11262" max="11262" width="30.7109375" style="3" customWidth="1"/>
-    <col min="11263" max="11264" width="9.140625" style="3" customWidth="1"/>
-    <col min="11265" max="11265" width="21.5703125" style="3" customWidth="1"/>
-    <col min="11266" max="11266" width="11.5703125" style="3" customWidth="1"/>
-    <col min="11267" max="11267" width="10.5703125" style="3" customWidth="1"/>
-    <col min="11268" max="11268" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11269" max="11513" width="8.85546875" style="3"/>
-    <col min="11514" max="11514" width="4.7109375" style="3" customWidth="1"/>
-    <col min="11515" max="11515" width="5.28515625" style="3" customWidth="1"/>
-    <col min="11516" max="11516" width="6.85546875" style="3" customWidth="1"/>
+    <col min="11262" max="11262" width="30.6640625" style="3" customWidth="1"/>
+    <col min="11263" max="11264" width="9.109375" style="3" customWidth="1"/>
+    <col min="11265" max="11265" width="21.5546875" style="3" customWidth="1"/>
+    <col min="11266" max="11266" width="11.5546875" style="3" customWidth="1"/>
+    <col min="11267" max="11267" width="10.5546875" style="3" customWidth="1"/>
+    <col min="11268" max="11268" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11269" max="11513" width="8.88671875" style="3"/>
+    <col min="11514" max="11514" width="4.6640625" style="3" customWidth="1"/>
+    <col min="11515" max="11515" width="5.33203125" style="3" customWidth="1"/>
+    <col min="11516" max="11516" width="6.88671875" style="3" customWidth="1"/>
     <col min="11517" max="11517" width="18" style="3" customWidth="1"/>
-    <col min="11518" max="11518" width="30.7109375" style="3" customWidth="1"/>
-    <col min="11519" max="11520" width="9.140625" style="3" customWidth="1"/>
-    <col min="11521" max="11521" width="21.5703125" style="3" customWidth="1"/>
-    <col min="11522" max="11522" width="11.5703125" style="3" customWidth="1"/>
-    <col min="11523" max="11523" width="10.5703125" style="3" customWidth="1"/>
-    <col min="11524" max="11524" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11525" max="11769" width="8.85546875" style="3"/>
-    <col min="11770" max="11770" width="4.7109375" style="3" customWidth="1"/>
-    <col min="11771" max="11771" width="5.28515625" style="3" customWidth="1"/>
-    <col min="11772" max="11772" width="6.85546875" style="3" customWidth="1"/>
+    <col min="11518" max="11518" width="30.6640625" style="3" customWidth="1"/>
+    <col min="11519" max="11520" width="9.109375" style="3" customWidth="1"/>
+    <col min="11521" max="11521" width="21.5546875" style="3" customWidth="1"/>
+    <col min="11522" max="11522" width="11.5546875" style="3" customWidth="1"/>
+    <col min="11523" max="11523" width="10.5546875" style="3" customWidth="1"/>
+    <col min="11524" max="11524" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11525" max="11769" width="8.88671875" style="3"/>
+    <col min="11770" max="11770" width="4.6640625" style="3" customWidth="1"/>
+    <col min="11771" max="11771" width="5.33203125" style="3" customWidth="1"/>
+    <col min="11772" max="11772" width="6.88671875" style="3" customWidth="1"/>
     <col min="11773" max="11773" width="18" style="3" customWidth="1"/>
-    <col min="11774" max="11774" width="30.7109375" style="3" customWidth="1"/>
-    <col min="11775" max="11776" width="9.140625" style="3" customWidth="1"/>
-    <col min="11777" max="11777" width="21.5703125" style="3" customWidth="1"/>
-    <col min="11778" max="11778" width="11.5703125" style="3" customWidth="1"/>
-    <col min="11779" max="11779" width="10.5703125" style="3" customWidth="1"/>
-    <col min="11780" max="11780" width="12.28515625" style="3" customWidth="1"/>
-    <col min="11781" max="12025" width="8.85546875" style="3"/>
-    <col min="12026" max="12026" width="4.7109375" style="3" customWidth="1"/>
-    <col min="12027" max="12027" width="5.28515625" style="3" customWidth="1"/>
-    <col min="12028" max="12028" width="6.85546875" style="3" customWidth="1"/>
+    <col min="11774" max="11774" width="30.6640625" style="3" customWidth="1"/>
+    <col min="11775" max="11776" width="9.109375" style="3" customWidth="1"/>
+    <col min="11777" max="11777" width="21.5546875" style="3" customWidth="1"/>
+    <col min="11778" max="11778" width="11.5546875" style="3" customWidth="1"/>
+    <col min="11779" max="11779" width="10.5546875" style="3" customWidth="1"/>
+    <col min="11780" max="11780" width="12.33203125" style="3" customWidth="1"/>
+    <col min="11781" max="12025" width="8.88671875" style="3"/>
+    <col min="12026" max="12026" width="4.6640625" style="3" customWidth="1"/>
+    <col min="12027" max="12027" width="5.33203125" style="3" customWidth="1"/>
+    <col min="12028" max="12028" width="6.88671875" style="3" customWidth="1"/>
     <col min="12029" max="12029" width="18" style="3" customWidth="1"/>
-    <col min="12030" max="12030" width="30.7109375" style="3" customWidth="1"/>
-    <col min="12031" max="12032" width="9.140625" style="3" customWidth="1"/>
-    <col min="12033" max="12033" width="21.5703125" style="3" customWidth="1"/>
-    <col min="12034" max="12034" width="11.5703125" style="3" customWidth="1"/>
-    <col min="12035" max="12035" width="10.5703125" style="3" customWidth="1"/>
-    <col min="12036" max="12036" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12037" max="12281" width="8.85546875" style="3"/>
-    <col min="12282" max="12282" width="4.7109375" style="3" customWidth="1"/>
-    <col min="12283" max="12283" width="5.28515625" style="3" customWidth="1"/>
-    <col min="12284" max="12284" width="6.85546875" style="3" customWidth="1"/>
+    <col min="12030" max="12030" width="30.6640625" style="3" customWidth="1"/>
+    <col min="12031" max="12032" width="9.109375" style="3" customWidth="1"/>
+    <col min="12033" max="12033" width="21.5546875" style="3" customWidth="1"/>
+    <col min="12034" max="12034" width="11.5546875" style="3" customWidth="1"/>
+    <col min="12035" max="12035" width="10.5546875" style="3" customWidth="1"/>
+    <col min="12036" max="12036" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12037" max="12281" width="8.88671875" style="3"/>
+    <col min="12282" max="12282" width="4.6640625" style="3" customWidth="1"/>
+    <col min="12283" max="12283" width="5.33203125" style="3" customWidth="1"/>
+    <col min="12284" max="12284" width="6.88671875" style="3" customWidth="1"/>
     <col min="12285" max="12285" width="18" style="3" customWidth="1"/>
-    <col min="12286" max="12286" width="30.7109375" style="3" customWidth="1"/>
-    <col min="12287" max="12288" width="9.140625" style="3" customWidth="1"/>
-    <col min="12289" max="12289" width="21.5703125" style="3" customWidth="1"/>
-    <col min="12290" max="12290" width="11.5703125" style="3" customWidth="1"/>
-    <col min="12291" max="12291" width="10.5703125" style="3" customWidth="1"/>
-    <col min="12292" max="12292" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12293" max="12537" width="8.85546875" style="3"/>
-    <col min="12538" max="12538" width="4.7109375" style="3" customWidth="1"/>
-    <col min="12539" max="12539" width="5.28515625" style="3" customWidth="1"/>
-    <col min="12540" max="12540" width="6.85546875" style="3" customWidth="1"/>
+    <col min="12286" max="12286" width="30.6640625" style="3" customWidth="1"/>
+    <col min="12287" max="12288" width="9.109375" style="3" customWidth="1"/>
+    <col min="12289" max="12289" width="21.5546875" style="3" customWidth="1"/>
+    <col min="12290" max="12290" width="11.5546875" style="3" customWidth="1"/>
+    <col min="12291" max="12291" width="10.5546875" style="3" customWidth="1"/>
+    <col min="12292" max="12292" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12293" max="12537" width="8.88671875" style="3"/>
+    <col min="12538" max="12538" width="4.6640625" style="3" customWidth="1"/>
+    <col min="12539" max="12539" width="5.33203125" style="3" customWidth="1"/>
+    <col min="12540" max="12540" width="6.88671875" style="3" customWidth="1"/>
     <col min="12541" max="12541" width="18" style="3" customWidth="1"/>
-    <col min="12542" max="12542" width="30.7109375" style="3" customWidth="1"/>
-    <col min="12543" max="12544" width="9.140625" style="3" customWidth="1"/>
-    <col min="12545" max="12545" width="21.5703125" style="3" customWidth="1"/>
-    <col min="12546" max="12546" width="11.5703125" style="3" customWidth="1"/>
-    <col min="12547" max="12547" width="10.5703125" style="3" customWidth="1"/>
-    <col min="12548" max="12548" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12549" max="12793" width="8.85546875" style="3"/>
-    <col min="12794" max="12794" width="4.7109375" style="3" customWidth="1"/>
-    <col min="12795" max="12795" width="5.28515625" style="3" customWidth="1"/>
-    <col min="12796" max="12796" width="6.85546875" style="3" customWidth="1"/>
+    <col min="12542" max="12542" width="30.6640625" style="3" customWidth="1"/>
+    <col min="12543" max="12544" width="9.109375" style="3" customWidth="1"/>
+    <col min="12545" max="12545" width="21.5546875" style="3" customWidth="1"/>
+    <col min="12546" max="12546" width="11.5546875" style="3" customWidth="1"/>
+    <col min="12547" max="12547" width="10.5546875" style="3" customWidth="1"/>
+    <col min="12548" max="12548" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12549" max="12793" width="8.88671875" style="3"/>
+    <col min="12794" max="12794" width="4.6640625" style="3" customWidth="1"/>
+    <col min="12795" max="12795" width="5.33203125" style="3" customWidth="1"/>
+    <col min="12796" max="12796" width="6.88671875" style="3" customWidth="1"/>
     <col min="12797" max="12797" width="18" style="3" customWidth="1"/>
-    <col min="12798" max="12798" width="30.7109375" style="3" customWidth="1"/>
-    <col min="12799" max="12800" width="9.140625" style="3" customWidth="1"/>
-    <col min="12801" max="12801" width="21.5703125" style="3" customWidth="1"/>
-    <col min="12802" max="12802" width="11.5703125" style="3" customWidth="1"/>
-    <col min="12803" max="12803" width="10.5703125" style="3" customWidth="1"/>
-    <col min="12804" max="12804" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12805" max="13049" width="8.85546875" style="3"/>
-    <col min="13050" max="13050" width="4.7109375" style="3" customWidth="1"/>
-    <col min="13051" max="13051" width="5.28515625" style="3" customWidth="1"/>
-    <col min="13052" max="13052" width="6.85546875" style="3" customWidth="1"/>
+    <col min="12798" max="12798" width="30.6640625" style="3" customWidth="1"/>
+    <col min="12799" max="12800" width="9.109375" style="3" customWidth="1"/>
+    <col min="12801" max="12801" width="21.5546875" style="3" customWidth="1"/>
+    <col min="12802" max="12802" width="11.5546875" style="3" customWidth="1"/>
+    <col min="12803" max="12803" width="10.5546875" style="3" customWidth="1"/>
+    <col min="12804" max="12804" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12805" max="13049" width="8.88671875" style="3"/>
+    <col min="13050" max="13050" width="4.6640625" style="3" customWidth="1"/>
+    <col min="13051" max="13051" width="5.33203125" style="3" customWidth="1"/>
+    <col min="13052" max="13052" width="6.88671875" style="3" customWidth="1"/>
     <col min="13053" max="13053" width="18" style="3" customWidth="1"/>
-    <col min="13054" max="13054" width="30.7109375" style="3" customWidth="1"/>
-    <col min="13055" max="13056" width="9.140625" style="3" customWidth="1"/>
-    <col min="13057" max="13057" width="21.5703125" style="3" customWidth="1"/>
-    <col min="13058" max="13058" width="11.5703125" style="3" customWidth="1"/>
-    <col min="13059" max="13059" width="10.5703125" style="3" customWidth="1"/>
-    <col min="13060" max="13060" width="12.28515625" style="3" customWidth="1"/>
-    <col min="13061" max="13305" width="8.85546875" style="3"/>
-    <col min="13306" max="13306" width="4.7109375" style="3" customWidth="1"/>
-    <col min="13307" max="13307" width="5.28515625" style="3" customWidth="1"/>
-    <col min="13308" max="13308" width="6.85546875" style="3" customWidth="1"/>
+    <col min="13054" max="13054" width="30.6640625" style="3" customWidth="1"/>
+    <col min="13055" max="13056" width="9.109375" style="3" customWidth="1"/>
+    <col min="13057" max="13057" width="21.5546875" style="3" customWidth="1"/>
+    <col min="13058" max="13058" width="11.5546875" style="3" customWidth="1"/>
+    <col min="13059" max="13059" width="10.5546875" style="3" customWidth="1"/>
+    <col min="13060" max="13060" width="12.33203125" style="3" customWidth="1"/>
+    <col min="13061" max="13305" width="8.88671875" style="3"/>
+    <col min="13306" max="13306" width="4.6640625" style="3" customWidth="1"/>
+    <col min="13307" max="13307" width="5.33203125" style="3" customWidth="1"/>
+    <col min="13308" max="13308" width="6.88671875" style="3" customWidth="1"/>
     <col min="13309" max="13309" width="18" style="3" customWidth="1"/>
-    <col min="13310" max="13310" width="30.7109375" style="3" customWidth="1"/>
-    <col min="13311" max="13312" width="9.140625" style="3" customWidth="1"/>
-    <col min="13313" max="13313" width="21.5703125" style="3" customWidth="1"/>
-    <col min="13314" max="13314" width="11.5703125" style="3" customWidth="1"/>
-    <col min="13315" max="13315" width="10.5703125" style="3" customWidth="1"/>
-    <col min="13316" max="13316" width="12.28515625" style="3" customWidth="1"/>
-    <col min="13317" max="13561" width="8.85546875" style="3"/>
-    <col min="13562" max="13562" width="4.7109375" style="3" customWidth="1"/>
-    <col min="13563" max="13563" width="5.28515625" style="3" customWidth="1"/>
-    <col min="13564" max="13564" width="6.85546875" style="3" customWidth="1"/>
+    <col min="13310" max="13310" width="30.6640625" style="3" customWidth="1"/>
+    <col min="13311" max="13312" width="9.109375" style="3" customWidth="1"/>
+    <col min="13313" max="13313" width="21.5546875" style="3" customWidth="1"/>
+    <col min="13314" max="13314" width="11.5546875" style="3" customWidth="1"/>
+    <col min="13315" max="13315" width="10.5546875" style="3" customWidth="1"/>
+    <col min="13316" max="13316" width="12.33203125" style="3" customWidth="1"/>
+    <col min="13317" max="13561" width="8.88671875" style="3"/>
+    <col min="13562" max="13562" width="4.6640625" style="3" customWidth="1"/>
+    <col min="13563" max="13563" width="5.33203125" style="3" customWidth="1"/>
+    <col min="13564" max="13564" width="6.88671875" style="3" customWidth="1"/>
     <col min="13565" max="13565" width="18" style="3" customWidth="1"/>
-    <col min="13566" max="13566" width="30.7109375" style="3" customWidth="1"/>
-    <col min="13567" max="13568" width="9.140625" style="3" customWidth="1"/>
-    <col min="13569" max="13569" width="21.5703125" style="3" customWidth="1"/>
-    <col min="13570" max="13570" width="11.5703125" style="3" customWidth="1"/>
-    <col min="13571" max="13571" width="10.5703125" style="3" customWidth="1"/>
-    <col min="13572" max="13572" width="12.28515625" style="3" customWidth="1"/>
-    <col min="13573" max="13817" width="8.85546875" style="3"/>
-    <col min="13818" max="13818" width="4.7109375" style="3" customWidth="1"/>
-    <col min="13819" max="13819" width="5.28515625" style="3" customWidth="1"/>
-    <col min="13820" max="13820" width="6.85546875" style="3" customWidth="1"/>
+    <col min="13566" max="13566" width="30.6640625" style="3" customWidth="1"/>
+    <col min="13567" max="13568" width="9.109375" style="3" customWidth="1"/>
+    <col min="13569" max="13569" width="21.5546875" style="3" customWidth="1"/>
+    <col min="13570" max="13570" width="11.5546875" style="3" customWidth="1"/>
+    <col min="13571" max="13571" width="10.5546875" style="3" customWidth="1"/>
+    <col min="13572" max="13572" width="12.33203125" style="3" customWidth="1"/>
+    <col min="13573" max="13817" width="8.88671875" style="3"/>
+    <col min="13818" max="13818" width="4.6640625" style="3" customWidth="1"/>
+    <col min="13819" max="13819" width="5.33203125" style="3" customWidth="1"/>
+    <col min="13820" max="13820" width="6.88671875" style="3" customWidth="1"/>
     <col min="13821" max="13821" width="18" style="3" customWidth="1"/>
-    <col min="13822" max="13822" width="30.7109375" style="3" customWidth="1"/>
-    <col min="13823" max="13824" width="9.140625" style="3" customWidth="1"/>
-    <col min="13825" max="13825" width="21.5703125" style="3" customWidth="1"/>
-    <col min="13826" max="13826" width="11.5703125" style="3" customWidth="1"/>
-    <col min="13827" max="13827" width="10.5703125" style="3" customWidth="1"/>
-    <col min="13828" max="13828" width="12.28515625" style="3" customWidth="1"/>
-    <col min="13829" max="14073" width="8.85546875" style="3"/>
-    <col min="14074" max="14074" width="4.7109375" style="3" customWidth="1"/>
-    <col min="14075" max="14075" width="5.28515625" style="3" customWidth="1"/>
-    <col min="14076" max="14076" width="6.85546875" style="3" customWidth="1"/>
+    <col min="13822" max="13822" width="30.6640625" style="3" customWidth="1"/>
+    <col min="13823" max="13824" width="9.109375" style="3" customWidth="1"/>
+    <col min="13825" max="13825" width="21.5546875" style="3" customWidth="1"/>
+    <col min="13826" max="13826" width="11.5546875" style="3" customWidth="1"/>
+    <col min="13827" max="13827" width="10.5546875" style="3" customWidth="1"/>
+    <col min="13828" max="13828" width="12.33203125" style="3" customWidth="1"/>
+    <col min="13829" max="14073" width="8.88671875" style="3"/>
+    <col min="14074" max="14074" width="4.6640625" style="3" customWidth="1"/>
+    <col min="14075" max="14075" width="5.33203125" style="3" customWidth="1"/>
+    <col min="14076" max="14076" width="6.88671875" style="3" customWidth="1"/>
     <col min="14077" max="14077" width="18" style="3" customWidth="1"/>
-    <col min="14078" max="14078" width="30.7109375" style="3" customWidth="1"/>
-    <col min="14079" max="14080" width="9.140625" style="3" customWidth="1"/>
-    <col min="14081" max="14081" width="21.5703125" style="3" customWidth="1"/>
-    <col min="14082" max="14082" width="11.5703125" style="3" customWidth="1"/>
-    <col min="14083" max="14083" width="10.5703125" style="3" customWidth="1"/>
-    <col min="14084" max="14084" width="12.28515625" style="3" customWidth="1"/>
-    <col min="14085" max="14329" width="8.85546875" style="3"/>
-    <col min="14330" max="14330" width="4.7109375" style="3" customWidth="1"/>
-    <col min="14331" max="14331" width="5.28515625" style="3" customWidth="1"/>
-    <col min="14332" max="14332" width="6.85546875" style="3" customWidth="1"/>
+    <col min="14078" max="14078" width="30.6640625" style="3" customWidth="1"/>
+    <col min="14079" max="14080" width="9.109375" style="3" customWidth="1"/>
+    <col min="14081" max="14081" width="21.5546875" style="3" customWidth="1"/>
+    <col min="14082" max="14082" width="11.5546875" style="3" customWidth="1"/>
+    <col min="14083" max="14083" width="10.5546875" style="3" customWidth="1"/>
+    <col min="14084" max="14084" width="12.33203125" style="3" customWidth="1"/>
+    <col min="14085" max="14329" width="8.88671875" style="3"/>
+    <col min="14330" max="14330" width="4.6640625" style="3" customWidth="1"/>
+    <col min="14331" max="14331" width="5.33203125" style="3" customWidth="1"/>
+    <col min="14332" max="14332" width="6.88671875" style="3" customWidth="1"/>
     <col min="14333" max="14333" width="18" style="3" customWidth="1"/>
-    <col min="14334" max="14334" width="30.7109375" style="3" customWidth="1"/>
-    <col min="14335" max="14336" width="9.140625" style="3" customWidth="1"/>
-    <col min="14337" max="14337" width="21.5703125" style="3" customWidth="1"/>
-    <col min="14338" max="14338" width="11.5703125" style="3" customWidth="1"/>
-    <col min="14339" max="14339" width="10.5703125" style="3" customWidth="1"/>
-    <col min="14340" max="14340" width="12.28515625" style="3" customWidth="1"/>
-    <col min="14341" max="14585" width="8.85546875" style="3"/>
-    <col min="14586" max="14586" width="4.7109375" style="3" customWidth="1"/>
-    <col min="14587" max="14587" width="5.28515625" style="3" customWidth="1"/>
-    <col min="14588" max="14588" width="6.85546875" style="3" customWidth="1"/>
+    <col min="14334" max="14334" width="30.6640625" style="3" customWidth="1"/>
+    <col min="14335" max="14336" width="9.109375" style="3" customWidth="1"/>
+    <col min="14337" max="14337" width="21.5546875" style="3" customWidth="1"/>
+    <col min="14338" max="14338" width="11.5546875" style="3" customWidth="1"/>
+    <col min="14339" max="14339" width="10.5546875" style="3" customWidth="1"/>
+    <col min="14340" max="14340" width="12.33203125" style="3" customWidth="1"/>
+    <col min="14341" max="14585" width="8.88671875" style="3"/>
+    <col min="14586" max="14586" width="4.6640625" style="3" customWidth="1"/>
+    <col min="14587" max="14587" width="5.33203125" style="3" customWidth="1"/>
+    <col min="14588" max="14588" width="6.88671875" style="3" customWidth="1"/>
     <col min="14589" max="14589" width="18" style="3" customWidth="1"/>
-    <col min="14590" max="14590" width="30.7109375" style="3" customWidth="1"/>
-    <col min="14591" max="14592" width="9.140625" style="3" customWidth="1"/>
-    <col min="14593" max="14593" width="21.5703125" style="3" customWidth="1"/>
-    <col min="14594" max="14594" width="11.5703125" style="3" customWidth="1"/>
-    <col min="14595" max="14595" width="10.5703125" style="3" customWidth="1"/>
-    <col min="14596" max="14596" width="12.28515625" style="3" customWidth="1"/>
-    <col min="14597" max="14841" width="8.85546875" style="3"/>
-    <col min="14842" max="14842" width="4.7109375" style="3" customWidth="1"/>
-    <col min="14843" max="14843" width="5.28515625" style="3" customWidth="1"/>
-    <col min="14844" max="14844" width="6.85546875" style="3" customWidth="1"/>
+    <col min="14590" max="14590" width="30.6640625" style="3" customWidth="1"/>
+    <col min="14591" max="14592" width="9.109375" style="3" customWidth="1"/>
+    <col min="14593" max="14593" width="21.5546875" style="3" customWidth="1"/>
+    <col min="14594" max="14594" width="11.5546875" style="3" customWidth="1"/>
+    <col min="14595" max="14595" width="10.5546875" style="3" customWidth="1"/>
+    <col min="14596" max="14596" width="12.33203125" style="3" customWidth="1"/>
+    <col min="14597" max="14841" width="8.88671875" style="3"/>
+    <col min="14842" max="14842" width="4.6640625" style="3" customWidth="1"/>
+    <col min="14843" max="14843" width="5.33203125" style="3" customWidth="1"/>
+    <col min="14844" max="14844" width="6.88671875" style="3" customWidth="1"/>
     <col min="14845" max="14845" width="18" style="3" customWidth="1"/>
-    <col min="14846" max="14846" width="30.7109375" style="3" customWidth="1"/>
-    <col min="14847" max="14848" width="9.140625" style="3" customWidth="1"/>
-    <col min="14849" max="14849" width="21.5703125" style="3" customWidth="1"/>
-    <col min="14850" max="14850" width="11.5703125" style="3" customWidth="1"/>
-    <col min="14851" max="14851" width="10.5703125" style="3" customWidth="1"/>
-    <col min="14852" max="14852" width="12.28515625" style="3" customWidth="1"/>
-    <col min="14853" max="15097" width="8.85546875" style="3"/>
-    <col min="15098" max="15098" width="4.7109375" style="3" customWidth="1"/>
-    <col min="15099" max="15099" width="5.28515625" style="3" customWidth="1"/>
-    <col min="15100" max="15100" width="6.85546875" style="3" customWidth="1"/>
+    <col min="14846" max="14846" width="30.6640625" style="3" customWidth="1"/>
+    <col min="14847" max="14848" width="9.109375" style="3" customWidth="1"/>
+    <col min="14849" max="14849" width="21.5546875" style="3" customWidth="1"/>
+    <col min="14850" max="14850" width="11.5546875" style="3" customWidth="1"/>
+    <col min="14851" max="14851" width="10.5546875" style="3" customWidth="1"/>
+    <col min="14852" max="14852" width="12.33203125" style="3" customWidth="1"/>
+    <col min="14853" max="15097" width="8.88671875" style="3"/>
+    <col min="15098" max="15098" width="4.6640625" style="3" customWidth="1"/>
+    <col min="15099" max="15099" width="5.33203125" style="3" customWidth="1"/>
+    <col min="15100" max="15100" width="6.88671875" style="3" customWidth="1"/>
     <col min="15101" max="15101" width="18" style="3" customWidth="1"/>
-    <col min="15102" max="15102" width="30.7109375" style="3" customWidth="1"/>
-    <col min="15103" max="15104" width="9.140625" style="3" customWidth="1"/>
-    <col min="15105" max="15105" width="21.5703125" style="3" customWidth="1"/>
-    <col min="15106" max="15106" width="11.5703125" style="3" customWidth="1"/>
-    <col min="15107" max="15107" width="10.5703125" style="3" customWidth="1"/>
-    <col min="15108" max="15108" width="12.28515625" style="3" customWidth="1"/>
-    <col min="15109" max="15353" width="8.85546875" style="3"/>
-    <col min="15354" max="15354" width="4.7109375" style="3" customWidth="1"/>
-    <col min="15355" max="15355" width="5.28515625" style="3" customWidth="1"/>
-    <col min="15356" max="15356" width="6.85546875" style="3" customWidth="1"/>
+    <col min="15102" max="15102" width="30.6640625" style="3" customWidth="1"/>
+    <col min="15103" max="15104" width="9.109375" style="3" customWidth="1"/>
+    <col min="15105" max="15105" width="21.5546875" style="3" customWidth="1"/>
+    <col min="15106" max="15106" width="11.5546875" style="3" customWidth="1"/>
+    <col min="15107" max="15107" width="10.5546875" style="3" customWidth="1"/>
+    <col min="15108" max="15108" width="12.33203125" style="3" customWidth="1"/>
+    <col min="15109" max="15353" width="8.88671875" style="3"/>
+    <col min="15354" max="15354" width="4.6640625" style="3" customWidth="1"/>
+    <col min="15355" max="15355" width="5.33203125" style="3" customWidth="1"/>
+    <col min="15356" max="15356" width="6.88671875" style="3" customWidth="1"/>
     <col min="15357" max="15357" width="18" style="3" customWidth="1"/>
-    <col min="15358" max="15358" width="30.7109375" style="3" customWidth="1"/>
-    <col min="15359" max="15360" width="9.140625" style="3" customWidth="1"/>
-    <col min="15361" max="15361" width="21.5703125" style="3" customWidth="1"/>
-    <col min="15362" max="15362" width="11.5703125" style="3" customWidth="1"/>
-    <col min="15363" max="15363" width="10.5703125" style="3" customWidth="1"/>
-    <col min="15364" max="15364" width="12.28515625" style="3" customWidth="1"/>
-    <col min="15365" max="15609" width="8.85546875" style="3"/>
-    <col min="15610" max="15610" width="4.7109375" style="3" customWidth="1"/>
-    <col min="15611" max="15611" width="5.28515625" style="3" customWidth="1"/>
-    <col min="15612" max="15612" width="6.85546875" style="3" customWidth="1"/>
+    <col min="15358" max="15358" width="30.6640625" style="3" customWidth="1"/>
+    <col min="15359" max="15360" width="9.109375" style="3" customWidth="1"/>
+    <col min="15361" max="15361" width="21.5546875" style="3" customWidth="1"/>
+    <col min="15362" max="15362" width="11.5546875" style="3" customWidth="1"/>
+    <col min="15363" max="15363" width="10.5546875" style="3" customWidth="1"/>
+    <col min="15364" max="15364" width="12.33203125" style="3" customWidth="1"/>
+    <col min="15365" max="15609" width="8.88671875" style="3"/>
+    <col min="15610" max="15610" width="4.6640625" style="3" customWidth="1"/>
+    <col min="15611" max="15611" width="5.33203125" style="3" customWidth="1"/>
+    <col min="15612" max="15612" width="6.88671875" style="3" customWidth="1"/>
     <col min="15613" max="15613" width="18" style="3" customWidth="1"/>
-    <col min="15614" max="15614" width="30.7109375" style="3" customWidth="1"/>
-    <col min="15615" max="15616" width="9.140625" style="3" customWidth="1"/>
-    <col min="15617" max="15617" width="21.5703125" style="3" customWidth="1"/>
-    <col min="15618" max="15618" width="11.5703125" style="3" customWidth="1"/>
-    <col min="15619" max="15619" width="10.5703125" style="3" customWidth="1"/>
-    <col min="15620" max="15620" width="12.28515625" style="3" customWidth="1"/>
-    <col min="15621" max="15865" width="8.85546875" style="3"/>
-    <col min="15866" max="15866" width="4.7109375" style="3" customWidth="1"/>
-    <col min="15867" max="15867" width="5.28515625" style="3" customWidth="1"/>
-    <col min="15868" max="15868" width="6.85546875" style="3" customWidth="1"/>
+    <col min="15614" max="15614" width="30.6640625" style="3" customWidth="1"/>
+    <col min="15615" max="15616" width="9.109375" style="3" customWidth="1"/>
+    <col min="15617" max="15617" width="21.5546875" style="3" customWidth="1"/>
+    <col min="15618" max="15618" width="11.5546875" style="3" customWidth="1"/>
+    <col min="15619" max="15619" width="10.5546875" style="3" customWidth="1"/>
+    <col min="15620" max="15620" width="12.33203125" style="3" customWidth="1"/>
+    <col min="15621" max="15865" width="8.88671875" style="3"/>
+    <col min="15866" max="15866" width="4.6640625" style="3" customWidth="1"/>
+    <col min="15867" max="15867" width="5.33203125" style="3" customWidth="1"/>
+    <col min="15868" max="15868" width="6.88671875" style="3" customWidth="1"/>
     <col min="15869" max="15869" width="18" style="3" customWidth="1"/>
-    <col min="15870" max="15870" width="30.7109375" style="3" customWidth="1"/>
-    <col min="15871" max="15872" width="9.140625" style="3" customWidth="1"/>
-    <col min="15873" max="15873" width="21.5703125" style="3" customWidth="1"/>
-    <col min="15874" max="15874" width="11.5703125" style="3" customWidth="1"/>
-    <col min="15875" max="15875" width="10.5703125" style="3" customWidth="1"/>
-    <col min="15876" max="15876" width="12.28515625" style="3" customWidth="1"/>
-    <col min="15877" max="16121" width="8.85546875" style="3"/>
-    <col min="16122" max="16122" width="4.7109375" style="3" customWidth="1"/>
-    <col min="16123" max="16123" width="5.28515625" style="3" customWidth="1"/>
-    <col min="16124" max="16124" width="6.85546875" style="3" customWidth="1"/>
+    <col min="15870" max="15870" width="30.6640625" style="3" customWidth="1"/>
+    <col min="15871" max="15872" width="9.109375" style="3" customWidth="1"/>
+    <col min="15873" max="15873" width="21.5546875" style="3" customWidth="1"/>
+    <col min="15874" max="15874" width="11.5546875" style="3" customWidth="1"/>
+    <col min="15875" max="15875" width="10.5546875" style="3" customWidth="1"/>
+    <col min="15876" max="15876" width="12.33203125" style="3" customWidth="1"/>
+    <col min="15877" max="16121" width="8.88671875" style="3"/>
+    <col min="16122" max="16122" width="4.6640625" style="3" customWidth="1"/>
+    <col min="16123" max="16123" width="5.33203125" style="3" customWidth="1"/>
+    <col min="16124" max="16124" width="6.88671875" style="3" customWidth="1"/>
     <col min="16125" max="16125" width="18" style="3" customWidth="1"/>
-    <col min="16126" max="16126" width="30.7109375" style="3" customWidth="1"/>
-    <col min="16127" max="16128" width="9.140625" style="3" customWidth="1"/>
-    <col min="16129" max="16129" width="21.5703125" style="3" customWidth="1"/>
-    <col min="16130" max="16130" width="11.5703125" style="3" customWidth="1"/>
-    <col min="16131" max="16131" width="10.5703125" style="3" customWidth="1"/>
-    <col min="16132" max="16132" width="12.28515625" style="3" customWidth="1"/>
-    <col min="16133" max="16374" width="8.85546875" style="3"/>
-    <col min="16375" max="16384" width="8.85546875" style="3" customWidth="1"/>
+    <col min="16126" max="16126" width="30.6640625" style="3" customWidth="1"/>
+    <col min="16127" max="16128" width="9.109375" style="3" customWidth="1"/>
+    <col min="16129" max="16129" width="21.5546875" style="3" customWidth="1"/>
+    <col min="16130" max="16130" width="11.5546875" style="3" customWidth="1"/>
+    <col min="16131" max="16131" width="10.5546875" style="3" customWidth="1"/>
+    <col min="16132" max="16132" width="12.33203125" style="3" customWidth="1"/>
+    <col min="16133" max="16374" width="8.88671875" style="3"/>
+    <col min="16375" max="16384" width="8.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:29" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-    </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
-    </row>
-    <row r="3" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
+    </row>
+    <row r="3" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42"/>
-    </row>
-    <row r="4" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="45"/>
+    </row>
+    <row r="4" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="44"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-    </row>
-    <row r="5" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="49"/>
+    </row>
+    <row r="5" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
-    </row>
-    <row r="6" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="43" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="Q6" s="30"/>
@@ -7938,23 +7944,23 @@
       <c r="AB6" s="30"/>
       <c r="AC6" s="30"/>
     </row>
-    <row r="7" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="46"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="49"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="Q7" s="30"/>
@@ -7971,25 +7977,25 @@
       <c r="AB7" s="30"/>
       <c r="AC7" s="30"/>
     </row>
-    <row r="8" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:29" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="Q8" s="30"/>
@@ -8006,19 +8012,19 @@
       <c r="AB8" s="30"/>
       <c r="AC8" s="30"/>
     </row>
-    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
+    <row r="9" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="Q9" s="30"/>
@@ -8035,33 +8041,33 @@
       <c r="AB9" s="30"/>
       <c r="AC9" s="30"/>
     </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+    <row r="10" spans="1:29" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="55" t="s">
+      <c r="K10" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="53" t="s">
+      <c r="L10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="32"/>
+      <c r="N10" s="55"/>
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="30"/>
@@ -8076,7 +8082,7 @@
       <c r="AB10" s="30"/>
       <c r="AC10" s="30"/>
     </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -8101,10 +8107,10 @@
       <c r="H11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="53"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="40"/>
       <c r="M11" s="17" t="s">
         <v>25</v>
       </c>
@@ -8125,13 +8131,9 @@
       <c r="AB11" s="30"/>
       <c r="AC11" s="30"/>
     </row>
-    <row r="12" spans="1:29" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
+    <row r="12" spans="1:29" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="12"/>
       <c r="D12" s="14"/>
       <c r="E12" s="26"/>
@@ -8149,11 +8151,9 @@
       <c r="N12" s="19"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:29" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
-      <c r="B13" s="11">
-        <v>2</v>
-      </c>
+      <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="14"/>
       <c r="E13" s="26"/>
@@ -8171,11 +8171,9 @@
       <c r="N13" s="19"/>
       <c r="O13" s="16"/>
     </row>
-    <row r="14" spans="1:29" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="11">
-        <v>3</v>
-      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="9"/>
       <c r="E14" s="26"/>
@@ -8193,11 +8191,9 @@
       <c r="N14" s="19"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:29" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="11">
-        <v>4</v>
-      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="14"/>
       <c r="E15" s="26"/>
@@ -8215,11 +8211,9 @@
       <c r="N15" s="19"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:29" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="11">
-        <v>5</v>
-      </c>
+      <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="14"/>
       <c r="E16" s="26"/>
@@ -8237,11 +8231,9 @@
       <c r="N16" s="19"/>
       <c r="O16" s="16"/>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="11">
-        <v>6</v>
-      </c>
+      <c r="B17" s="11"/>
       <c r="C17" s="12"/>
       <c r="D17" s="14"/>
       <c r="E17" s="26"/>
@@ -8259,11 +8251,9 @@
       <c r="N17" s="19"/>
       <c r="O17" s="16"/>
     </row>
-    <row r="18" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="11">
-        <v>7</v>
-      </c>
+      <c r="B18" s="11"/>
       <c r="C18" s="12"/>
       <c r="D18" s="14"/>
       <c r="E18" s="26"/>
@@ -8281,11 +8271,9 @@
       <c r="N18" s="19"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="11">
-        <v>8</v>
-      </c>
+      <c r="B19" s="11"/>
       <c r="C19" s="12"/>
       <c r="D19" s="14"/>
       <c r="E19" s="26"/>
@@ -8303,11 +8291,9 @@
       <c r="N19" s="19"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="11">
-        <v>9</v>
-      </c>
+      <c r="B20" s="11"/>
       <c r="C20" s="12"/>
       <c r="D20" s="14"/>
       <c r="E20" s="26"/>
@@ -8325,11 +8311,9 @@
       <c r="N20" s="19"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="11">
-        <v>10</v>
-      </c>
+      <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="14"/>
       <c r="E21" s="26"/>
@@ -8347,11 +8331,9 @@
       <c r="N21" s="19"/>
       <c r="O21" s="16"/>
     </row>
-    <row r="22" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="11">
-        <v>11</v>
-      </c>
+      <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="14"/>
       <c r="E22" s="26"/>
@@ -8369,11 +8351,9 @@
       <c r="N22" s="19"/>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="B23" s="11">
-        <v>12</v>
-      </c>
+      <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="14"/>
       <c r="E23" s="26"/>
@@ -8391,11 +8371,9 @@
       <c r="N23" s="19"/>
       <c r="O23" s="16"/>
     </row>
-    <row r="24" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="11">
-        <v>13</v>
-      </c>
+      <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="14"/>
       <c r="E24" s="26"/>
@@ -8413,11 +8391,9 @@
       <c r="N24" s="19"/>
       <c r="O24" s="16"/>
     </row>
-    <row r="25" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="11">
-        <v>14</v>
-      </c>
+      <c r="B25" s="11"/>
       <c r="C25" s="12"/>
       <c r="D25" s="14"/>
       <c r="E25" s="26"/>
@@ -8435,11 +8411,9 @@
       <c r="N25" s="19"/>
       <c r="O25" s="16"/>
     </row>
-    <row r="26" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="11">
-        <v>15</v>
-      </c>
+      <c r="B26" s="11"/>
       <c r="C26" s="12"/>
       <c r="D26" s="14"/>
       <c r="E26" s="26"/>
@@ -8457,11 +8431,9 @@
       <c r="N26" s="19"/>
       <c r="O26" s="16"/>
     </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="11">
-        <v>16</v>
-      </c>
+      <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="14"/>
       <c r="E27" s="26"/>
@@ -8479,11 +8451,9 @@
       <c r="N27" s="19"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="11">
-        <v>17</v>
-      </c>
+      <c r="B28" s="11"/>
       <c r="C28" s="12"/>
       <c r="D28" s="14"/>
       <c r="E28" s="26"/>
@@ -8501,7 +8471,7 @@
       <c r="N28" s="19"/>
       <c r="O28" s="16"/>
     </row>
-    <row r="29" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
@@ -8521,7 +8491,7 @@
       <c r="N29" s="19"/>
       <c r="O29" s="16"/>
     </row>
-    <row r="30" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
@@ -8541,7 +8511,7 @@
       <c r="N30" s="19"/>
       <c r="O30" s="16"/>
     </row>
-    <row r="31" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
@@ -8561,7 +8531,7 @@
       <c r="N31" s="19"/>
       <c r="O31" s="16"/>
     </row>
-    <row r="32" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12"/>
@@ -8580,7 +8550,7 @@
       <c r="N32" s="19"/>
       <c r="O32" s="16"/>
     </row>
-    <row r="33" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="12"/>
@@ -8600,7 +8570,7 @@
       <c r="N33" s="19"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="12"/>
@@ -8620,7 +8590,7 @@
       <c r="N34" s="19"/>
       <c r="O34" s="16"/>
     </row>
-    <row r="35" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="12"/>
@@ -8640,7 +8610,7 @@
       <c r="N35" s="19"/>
       <c r="O35" s="16"/>
     </row>
-    <row r="36" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="12"/>
@@ -8660,7 +8630,7 @@
       <c r="N36" s="19"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12"/>
@@ -8680,7 +8650,7 @@
       <c r="N37" s="19"/>
       <c r="O37" s="16"/>
     </row>
-    <row r="38" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
@@ -8700,7 +8670,7 @@
       <c r="N38" s="19"/>
       <c r="O38" s="16"/>
     </row>
-    <row r="39" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="12"/>
@@ -8720,7 +8690,7 @@
       <c r="N39" s="19"/>
       <c r="O39" s="16"/>
     </row>
-    <row r="40" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="12"/>
@@ -8740,7 +8710,7 @@
       <c r="N40" s="19"/>
       <c r="O40" s="16"/>
     </row>
-    <row r="41" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="12"/>
@@ -8760,7 +8730,7 @@
       <c r="N41" s="19"/>
       <c r="O41" s="16"/>
     </row>
-    <row r="42" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="12"/>
@@ -8780,7 +8750,7 @@
       <c r="N42" s="19"/>
       <c r="O42" s="16"/>
     </row>
-    <row r="43" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="12"/>
@@ -8800,7 +8770,7 @@
       <c r="N43" s="19"/>
       <c r="O43" s="16"/>
     </row>
-    <row r="44" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="12"/>
@@ -8820,7 +8790,7 @@
       <c r="N44" s="19"/>
       <c r="O44" s="16"/>
     </row>
-    <row r="45" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="12"/>
@@ -8840,7 +8810,7 @@
       <c r="N45" s="19"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
@@ -8859,7 +8829,7 @@
       <c r="N46" s="19"/>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
@@ -8879,7 +8849,7 @@
       <c r="N47" s="19"/>
       <c r="O47" s="16"/>
     </row>
-    <row r="48" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="12"/>
@@ -8899,7 +8869,7 @@
       <c r="N48" s="19"/>
       <c r="O48" s="16"/>
     </row>
-    <row r="49" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="12"/>
@@ -8919,7 +8889,7 @@
       <c r="N49" s="19"/>
       <c r="O49" s="16"/>
     </row>
-    <row r="50" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="12"/>
@@ -8939,7 +8909,7 @@
       <c r="N50" s="19"/>
       <c r="O50" s="16"/>
     </row>
-    <row r="51" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12"/>
@@ -8959,7 +8929,7 @@
       <c r="N51" s="19"/>
       <c r="O51" s="16"/>
     </row>
-    <row r="52" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="12"/>
@@ -8979,7 +8949,7 @@
       <c r="N52" s="19"/>
       <c r="O52" s="16"/>
     </row>
-    <row r="53" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
@@ -8999,7 +8969,7 @@
       <c r="N53" s="19"/>
       <c r="O53" s="16"/>
     </row>
-    <row r="54" spans="1:15" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" s="4" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
@@ -9019,778 +8989,751 @@
       <c r="N54" s="19"/>
       <c r="O54" s="16"/>
     </row>
-    <row r="55" spans="1:15" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="58" t="s">
+    <row r="55" spans="1:15" s="4" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="58"/>
-      <c r="C55" s="59" t="s">
+      <c r="B55" s="74"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="59"/>
-      <c r="L55" s="59"/>
-    </row>
-    <row r="56" spans="1:15" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="58"/>
-      <c r="B56" s="58"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="59"/>
-      <c r="K56" s="59"/>
-      <c r="L56" s="59"/>
-    </row>
-    <row r="57" spans="1:15" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
+      <c r="E55" s="72"/>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="72"/>
+      <c r="J55" s="72"/>
+      <c r="K55" s="72"/>
+      <c r="L55" s="73"/>
+    </row>
+    <row r="56" spans="1:15" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="56"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="62"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="60" t="s">
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="60"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="57"/>
-    </row>
-    <row r="58" spans="1:15" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="56" t="s">
+      <c r="H56" s="33"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="32"/>
+    </row>
+    <row r="57" spans="1:15" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="56"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="56" t="s">
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H58" s="56"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H57" s="31"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="32"/>
+    </row>
+    <row r="58" spans="1:15" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="9"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I59" s="1"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I60" s="1"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I61" s="1"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I62" s="1"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I63" s="1"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I64" s="1"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I65" s="1"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I66" s="1"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I67" s="1"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I68" s="1"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I69" s="1"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I70" s="1"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I71" s="1"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I72" s="1"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I73" s="1"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I74" s="1"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I75" s="1"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I76" s="1"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I77" s="1"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I78" s="1"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I79" s="1"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I80" s="1"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I81" s="1"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I82" s="1"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I83" s="1"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I84" s="1"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I85" s="1"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I86" s="1"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I87" s="1"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I88" s="1"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I89" s="1"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I90" s="1"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I91" s="1"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I92" s="1"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I93" s="1"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I94" s="1"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I95" s="1"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I96" s="1"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I97" s="1"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I98" s="1"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I99" s="1"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I100" s="1"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I101" s="1"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I102" s="1"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I103" s="1"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I104" s="1"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I105" s="1"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I106" s="1"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I107" s="1"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I108" s="1"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I109" s="1"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I110" s="1"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I111" s="1"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I112" s="1"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I113" s="1"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I114" s="1"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I115" s="1"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I116" s="1"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I117" s="1"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I118" s="1"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I119" s="1"/>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I120" s="1"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I121" s="1"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I122" s="1"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I123" s="1"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I124" s="1"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I125" s="1"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I126" s="1"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I127" s="1"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I128" s="1"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I129" s="1"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I130" s="1"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I131" s="1"/>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I132" s="1"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I133" s="1"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I134" s="1"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I135" s="1"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I136" s="1"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I137" s="1"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I138" s="1"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I139" s="1"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I140" s="1"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I141" s="1"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I142" s="1"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I143" s="1"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I144" s="1"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
     </row>
-    <row r="145" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I145" s="1"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
     </row>
-    <row r="146" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I146" s="1"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
     </row>
-    <row r="147" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I147" s="1"/>
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
     </row>
-    <row r="148" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I148" s="1"/>
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
     </row>
-    <row r="149" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I149" s="1"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
-    <row r="150" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I150" s="1"/>
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
     </row>
-    <row r="151" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I151" s="1"/>
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
     </row>
-    <row r="152" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I152" s="1"/>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
     </row>
-    <row r="153" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I153" s="1"/>
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
     </row>
-    <row r="154" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I154" s="1"/>
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I155" s="1"/>
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
     </row>
-    <row r="156" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I156" s="1"/>
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I157" s="1"/>
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I158" s="1"/>
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I159" s="1"/>
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
     </row>
-    <row r="160" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I160" s="1"/>
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
     </row>
-    <row r="161" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I161" s="1"/>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
     </row>
-    <row r="162" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I162" s="1"/>
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
     </row>
-    <row r="163" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I163" s="1"/>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
     </row>
-    <row r="164" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I164" s="1"/>
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
     </row>
-    <row r="165" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I165" s="1"/>
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
     </row>
-    <row r="166" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I166" s="1"/>
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
     </row>
-    <row r="167" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I167" s="1"/>
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
     </row>
-    <row r="168" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I168" s="1"/>
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
     </row>
-    <row r="169" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I169" s="1"/>
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
     </row>
-    <row r="170" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I170" s="1"/>
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>
     </row>
-    <row r="171" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I171" s="1"/>
       <c r="J171" s="2"/>
       <c r="K171" s="2"/>
     </row>
-    <row r="172" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I172" s="1"/>
       <c r="J172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I173" s="1"/>
       <c r="J173" s="2"/>
       <c r="K173" s="2"/>
     </row>
-    <row r="174" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I174" s="1"/>
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
     </row>
-    <row r="175" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I175" s="1"/>
       <c r="J175" s="2"/>
       <c r="K175" s="2"/>
     </row>
-    <row r="176" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I176" s="1"/>
       <c r="J176" s="2"/>
       <c r="K176" s="2"/>
     </row>
-    <row r="177" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I177" s="1"/>
       <c r="J177" s="2"/>
       <c r="K177" s="2"/>
     </row>
-    <row r="178" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I178" s="1"/>
       <c r="J178" s="2"/>
       <c r="K178" s="2"/>
     </row>
-    <row r="179" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I179" s="1"/>
       <c r="J179" s="2"/>
       <c r="K179" s="2"/>
     </row>
-    <row r="180" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I180" s="1"/>
       <c r="J180" s="2"/>
       <c r="K180" s="2"/>
     </row>
-    <row r="181" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I181" s="1"/>
-      <c r="J181" s="2"/>
-      <c r="K181" s="2"/>
-    </row>
-    <row r="182" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+    </row>
+    <row r="182" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I182" s="1"/>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
     </row>
-    <row r="183" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
     </row>
-    <row r="184" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
     </row>
-    <row r="185" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I185" s="1"/>
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
     </row>
-    <row r="186" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I186" s="1"/>
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
     </row>
-    <row r="187" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I187" s="1"/>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
     </row>
-    <row r="188" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I188" s="1"/>
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
     </row>
-    <row r="189" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I189" s="1"/>
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
     </row>
-    <row r="190" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I190" s="1"/>
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
     </row>
-    <row r="191" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I191" s="1"/>
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
     </row>
-    <row r="192" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I192" s="1"/>
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
     </row>
-    <row r="193" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I193" s="1"/>
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
     </row>
-    <row r="194" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I194" s="1"/>
-      <c r="J194" s="1"/>
-      <c r="K194" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:L58"/>
-    <mergeCell ref="A55:B56"/>
-    <mergeCell ref="C55:L56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:L57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A8:G8"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:D2"/>
@@ -9807,9 +9750,31 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:H6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I57:L57"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D55:L55"/>
+    <mergeCell ref="A55:C55"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
-  <conditionalFormatting sqref="L12:L54 L59:L129">
+  <conditionalFormatting sqref="L12:L54 L58:L128">
     <cfRule type="cellIs" dxfId="4" priority="426" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
@@ -9817,7 +9782,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:L132">
+  <conditionalFormatting sqref="L129:L131">
     <cfRule type="cellIs" dxfId="2" priority="428" stopIfTrue="1" operator="equal">
       <formula>"""Fail"""</formula>
     </cfRule>
@@ -9854,7 +9819,7 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9869,9 +9834,9 @@
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -9884,33 +9849,33 @@
       <c r="J1" s="22"/>
       <c r="K1" s="23"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -9923,7 +9888,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -9936,7 +9901,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -9949,7 +9914,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -9962,7 +9927,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -9975,7 +9940,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -9988,7 +9953,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -10001,7 +9966,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -10014,7 +9979,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -10027,7 +9992,7 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -10040,7 +10005,7 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -10053,7 +10018,7 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
@@ -10066,7 +10031,7 @@
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
@@ -10079,7 +10044,7 @@
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -10092,7 +10057,7 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -10105,7 +10070,7 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
@@ -10118,7 +10083,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -10131,7 +10096,7 @@
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -10144,7 +10109,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -10157,7 +10122,7 @@
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -10170,7 +10135,7 @@
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -10183,7 +10148,7 @@
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -10196,7 +10161,7 @@
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -10209,7 +10174,7 @@
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -10222,7 +10187,7 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -10235,7 +10200,7 @@
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -10248,7 +10213,7 @@
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
@@ -10261,7 +10226,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
@@ -10274,7 +10239,7 @@
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -10287,7 +10252,7 @@
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -10300,7 +10265,7 @@
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -10313,7 +10278,7 @@
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -10326,7 +10291,7 @@
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -10339,7 +10304,7 @@
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>

</xml_diff>